<commit_message>
Correct convolution layer backward phase
</commit_message>
<xml_diff>
--- a/Book2.xlsx
+++ b/Book2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\NeuralNetwork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DB4540FF-927E-4246-8277-8FFFD1DFB863}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{251E0D85-DAF1-4E3B-8171-3EF8245CCAE4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -568,8 +568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BN62"/>
   <sheetViews>
-    <sheetView topLeftCell="N28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AE58" sqref="AE58:BN58"/>
+    <sheetView topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AI4" sqref="AI4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2181,8 +2181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D771BA6-BDBF-4EDD-8045-037C0BFCFB28}">
   <dimension ref="A1:DH103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AP57" sqref="AP57:AP62"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AO4" sqref="AO4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2362,35 +2362,35 @@
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
       <c r="N3" s="6">
-        <f>SUMPRODUCT(B13:D15,$N$79:$P$81) + SUMPRODUCT(B2:D4,$N$73:$P$75) + SUMPRODUCT(B24:D26,$N$85:$P$87) + $S$73</f>
+        <f t="shared" ref="N3:U10" si="1">SUMPRODUCT(B13:D15,$N$79:$P$81) + SUMPRODUCT(B2:D4,$N$73:$P$75) + SUMPRODUCT(B24:D26,$N$85:$P$87) + $S$73</f>
         <v>55.000100000000003</v>
       </c>
       <c r="O3" s="6">
-        <f>SUMPRODUCT(C13:E15,$N$79:$P$81) + SUMPRODUCT(C2:E4,$N$73:$P$75) + SUMPRODUCT(C24:E26,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="P3" s="6">
-        <f>SUMPRODUCT(D13:F15,$N$79:$P$81) + SUMPRODUCT(D2:F4,$N$73:$P$75) + SUMPRODUCT(D24:F26,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="Q3" s="6">
-        <f>SUMPRODUCT(E13:G15,$N$79:$P$81) + SUMPRODUCT(E2:G4,$N$73:$P$75) + SUMPRODUCT(E24:G26,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="R3" s="6">
-        <f>SUMPRODUCT(F13:H15,$N$79:$P$81) + SUMPRODUCT(F2:H4,$N$73:$P$75) + SUMPRODUCT(F24:H26,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="S3" s="6">
-        <f>SUMPRODUCT(G13:I15,$N$79:$P$81) + SUMPRODUCT(G2:I4,$N$73:$P$75) + SUMPRODUCT(G24:I26,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="T3" s="6">
-        <f>SUMPRODUCT(H13:J15,$N$79:$P$81) + SUMPRODUCT(H2:J4,$N$73:$P$75) + SUMPRODUCT(H24:J26,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="U3" s="6">
-        <f>SUMPRODUCT(I13:K15,$N$79:$P$81) + SUMPRODUCT(I2:K4,$N$73:$P$75) + SUMPRODUCT(I24:K26,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="V3" s="6"/>
@@ -2413,7 +2413,7 @@
         <v>55.000099999999996</v>
       </c>
       <c r="AM3" s="1">
-        <f t="shared" ref="AM3:AM7" si="1">AC38</f>
+        <f t="shared" ref="AM3:AM7" si="2">AC38</f>
         <v>325.00109999999995</v>
       </c>
       <c r="AO3" s="1" t="s">
@@ -2461,35 +2461,35 @@
       <c r="L4" s="6"/>
       <c r="M4" s="6"/>
       <c r="N4" s="6">
-        <f>SUMPRODUCT(B14:D16,$N$79:$P$81) + SUMPRODUCT(B3:D5,$N$73:$P$75) + SUMPRODUCT(B25:D27,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="O4" s="6">
-        <f>SUMPRODUCT(C14:E16,$N$79:$P$81) + SUMPRODUCT(C3:E5,$N$73:$P$75) + SUMPRODUCT(C25:E27,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="P4" s="6">
-        <f>SUMPRODUCT(D14:F16,$N$79:$P$81) + SUMPRODUCT(D3:F5,$N$73:$P$75) + SUMPRODUCT(D25:F27,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="Q4" s="6">
-        <f>SUMPRODUCT(E14:G16,$N$79:$P$81) + SUMPRODUCT(E3:G5,$N$73:$P$75) + SUMPRODUCT(E25:G27,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="R4" s="6">
-        <f>SUMPRODUCT(F14:H16,$N$79:$P$81) + SUMPRODUCT(F3:H5,$N$73:$P$75) + SUMPRODUCT(F25:H27,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="S4" s="6">
-        <f>SUMPRODUCT(G14:I16,$N$79:$P$81) + SUMPRODUCT(G3:I5,$N$73:$P$75) + SUMPRODUCT(G25:I27,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="T4" s="6">
-        <f>SUMPRODUCT(H14:J16,$N$79:$P$81) + SUMPRODUCT(H3:J5,$N$73:$P$75) + SUMPRODUCT(H25:J27,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="U4" s="6">
-        <f>SUMPRODUCT(I14:K16,$N$79:$P$81) + SUMPRODUCT(I3:K5,$N$73:$P$75) + SUMPRODUCT(I25:K27,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="V4" s="6"/>
@@ -2500,27 +2500,27 @@
       <c r="AA4" s="7"/>
       <c r="AB4" s="5"/>
       <c r="AC4" s="6">
-        <f>SUMPRODUCT(N3:P5,$AC$73:$AE$75)</f>
+        <f t="shared" ref="AC4:AH9" si="3">SUMPRODUCT(N3:P5,$AC$73:$AE$75)</f>
         <v>55.000099999999996</v>
       </c>
       <c r="AD4" s="6">
-        <f>SUMPRODUCT(O3:Q5,$AC$73:$AE$75)</f>
+        <f t="shared" si="3"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AE4" s="6">
-        <f>SUMPRODUCT(P3:R5,$AC$73:$AE$75)</f>
+        <f t="shared" si="3"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AF4" s="6">
-        <f>SUMPRODUCT(Q3:S5,$AC$73:$AE$75)</f>
+        <f t="shared" si="3"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AG4" s="6">
-        <f>SUMPRODUCT(R3:T5,$AC$73:$AE$75)</f>
+        <f t="shared" si="3"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AH4" s="6">
-        <f>SUMPRODUCT(S3:U5,$AC$73:$AE$75)</f>
+        <f t="shared" si="3"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AI4" s="6"/>
@@ -2530,7 +2530,7 @@
         <v>55.000099999999996</v>
       </c>
       <c r="AM4" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>325.00109999999995</v>
       </c>
       <c r="AO4" s="1">
@@ -2590,35 +2590,35 @@
       <c r="L5" s="6"/>
       <c r="M5" s="6"/>
       <c r="N5" s="6">
-        <f>SUMPRODUCT(B15:D17,$N$79:$P$81) + SUMPRODUCT(B4:D6,$N$73:$P$75) + SUMPRODUCT(B26:D28,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="O5" s="6">
-        <f>SUMPRODUCT(C15:E17,$N$79:$P$81) + SUMPRODUCT(C4:E6,$N$73:$P$75) + SUMPRODUCT(C26:E28,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="P5" s="6">
-        <f>SUMPRODUCT(D15:F17,$N$79:$P$81) + SUMPRODUCT(D4:F6,$N$73:$P$75) + SUMPRODUCT(D26:F28,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="Q5" s="6">
-        <f>SUMPRODUCT(E15:G17,$N$79:$P$81) + SUMPRODUCT(E4:G6,$N$73:$P$75) + SUMPRODUCT(E26:G28,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="R5" s="6">
-        <f>SUMPRODUCT(F15:H17,$N$79:$P$81) + SUMPRODUCT(F4:H6,$N$73:$P$75) + SUMPRODUCT(F26:H28,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="S5" s="6">
-        <f>SUMPRODUCT(G15:I17,$N$79:$P$81) + SUMPRODUCT(G4:I6,$N$73:$P$75) + SUMPRODUCT(G26:I28,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="T5" s="6">
-        <f>SUMPRODUCT(H15:J17,$N$79:$P$81) + SUMPRODUCT(H4:J6,$N$73:$P$75) + SUMPRODUCT(H26:J28,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="U5" s="6">
-        <f>SUMPRODUCT(I15:K17,$N$79:$P$81) + SUMPRODUCT(I4:K6,$N$73:$P$75) + SUMPRODUCT(I26:K28,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="V5" s="6"/>
@@ -2629,27 +2629,27 @@
       <c r="AA5" s="7"/>
       <c r="AB5" s="5"/>
       <c r="AC5" s="6">
-        <f>SUMPRODUCT(N4:P6,$AC$73:$AE$75)</f>
+        <f t="shared" si="3"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AD5" s="6">
-        <f>SUMPRODUCT(O4:Q6,$AC$73:$AE$75)</f>
+        <f t="shared" si="3"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AE5" s="6">
-        <f>SUMPRODUCT(P4:R6,$AC$73:$AE$75)</f>
+        <f t="shared" si="3"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AF5" s="6">
-        <f>SUMPRODUCT(Q4:S6,$AC$73:$AE$75)</f>
+        <f t="shared" si="3"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AG5" s="6">
-        <f>SUMPRODUCT(R4:T6,$AC$73:$AE$75)</f>
+        <f t="shared" si="3"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AH5" s="6">
-        <f>SUMPRODUCT(S4:U6,$AC$73:$AE$75)</f>
+        <f t="shared" si="3"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AI5" s="6"/>
@@ -2659,7 +2659,7 @@
         <v>55.000099999999996</v>
       </c>
       <c r="AM5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>325.00109999999995</v>
       </c>
       <c r="AO5" s="1">
@@ -2718,35 +2718,35 @@
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
       <c r="N6" s="6">
-        <f>SUMPRODUCT(B16:D18,$N$79:$P$81) + SUMPRODUCT(B5:D7,$N$73:$P$75) + SUMPRODUCT(B27:D29,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="O6" s="6">
-        <f>SUMPRODUCT(C16:E18,$N$79:$P$81) + SUMPRODUCT(C5:E7,$N$73:$P$75) + SUMPRODUCT(C27:E29,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="P6" s="6">
-        <f>SUMPRODUCT(D16:F18,$N$79:$P$81) + SUMPRODUCT(D5:F7,$N$73:$P$75) + SUMPRODUCT(D27:F29,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="Q6" s="6">
-        <f>SUMPRODUCT(E16:G18,$N$79:$P$81) + SUMPRODUCT(E5:G7,$N$73:$P$75) + SUMPRODUCT(E27:G29,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="R6" s="6">
-        <f>SUMPRODUCT(F16:H18,$N$79:$P$81) + SUMPRODUCT(F5:H7,$N$73:$P$75) + SUMPRODUCT(F27:H29,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="S6" s="6">
-        <f>SUMPRODUCT(G16:I18,$N$79:$P$81) + SUMPRODUCT(G5:I7,$N$73:$P$75) + SUMPRODUCT(G27:I29,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="T6" s="6">
-        <f>SUMPRODUCT(H16:J18,$N$79:$P$81) + SUMPRODUCT(H5:J7,$N$73:$P$75) + SUMPRODUCT(H27:J29,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="U6" s="6">
-        <f>SUMPRODUCT(I16:K18,$N$79:$P$81) + SUMPRODUCT(I5:K7,$N$73:$P$75) + SUMPRODUCT(I27:K29,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="V6" s="6"/>
@@ -2757,27 +2757,27 @@
       <c r="AA6" s="7"/>
       <c r="AB6" s="5"/>
       <c r="AC6" s="6">
-        <f>SUMPRODUCT(N5:P7,$AC$73:$AE$75)</f>
+        <f t="shared" si="3"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AD6" s="6">
-        <f>SUMPRODUCT(O5:Q7,$AC$73:$AE$75)</f>
+        <f t="shared" si="3"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AE6" s="6">
-        <f>SUMPRODUCT(P5:R7,$AC$73:$AE$75)</f>
+        <f t="shared" si="3"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AF6" s="6">
-        <f>SUMPRODUCT(Q5:S7,$AC$73:$AE$75)</f>
+        <f t="shared" si="3"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AG6" s="6">
-        <f>SUMPRODUCT(R5:T7,$AC$73:$AE$75)</f>
+        <f t="shared" si="3"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AH6" s="6">
-        <f>SUMPRODUCT(S5:U7,$AC$73:$AE$75)</f>
+        <f t="shared" si="3"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AI6" s="6"/>
@@ -2787,7 +2787,7 @@
         <v>55.000099999999996</v>
       </c>
       <c r="AM6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>325.00109999999995</v>
       </c>
     </row>
@@ -2826,35 +2826,35 @@
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
       <c r="N7" s="6">
-        <f>SUMPRODUCT(B17:D19,$N$79:$P$81) + SUMPRODUCT(B6:D8,$N$73:$P$75) + SUMPRODUCT(B28:D30,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="O7" s="6">
-        <f>SUMPRODUCT(C17:E19,$N$79:$P$81) + SUMPRODUCT(C6:E8,$N$73:$P$75) + SUMPRODUCT(C28:E30,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="P7" s="6">
-        <f>SUMPRODUCT(D17:F19,$N$79:$P$81) + SUMPRODUCT(D6:F8,$N$73:$P$75) + SUMPRODUCT(D28:F30,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="Q7" s="6">
-        <f>SUMPRODUCT(E17:G19,$N$79:$P$81) + SUMPRODUCT(E6:G8,$N$73:$P$75) + SUMPRODUCT(E28:G30,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="R7" s="6">
-        <f>SUMPRODUCT(F17:H19,$N$79:$P$81) + SUMPRODUCT(F6:H8,$N$73:$P$75) + SUMPRODUCT(F28:H30,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="S7" s="6">
-        <f>SUMPRODUCT(G17:I19,$N$79:$P$81) + SUMPRODUCT(G6:I8,$N$73:$P$75) + SUMPRODUCT(G28:I30,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="T7" s="6">
-        <f>SUMPRODUCT(H17:J19,$N$79:$P$81) + SUMPRODUCT(H6:J8,$N$73:$P$75) + SUMPRODUCT(H28:J30,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="U7" s="6">
-        <f>SUMPRODUCT(I17:K19,$N$79:$P$81) + SUMPRODUCT(I6:K8,$N$73:$P$75) + SUMPRODUCT(I28:K30,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="V7" s="6"/>
@@ -2865,27 +2865,27 @@
       <c r="AA7" s="7"/>
       <c r="AB7" s="5"/>
       <c r="AC7" s="6">
-        <f>SUMPRODUCT(N6:P8,$AC$73:$AE$75)</f>
+        <f t="shared" si="3"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AD7" s="6">
-        <f>SUMPRODUCT(O6:Q8,$AC$73:$AE$75)</f>
+        <f t="shared" si="3"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AE7" s="6">
-        <f>SUMPRODUCT(P6:R8,$AC$73:$AE$75)</f>
+        <f t="shared" si="3"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AF7" s="6">
-        <f>SUMPRODUCT(Q6:S8,$AC$73:$AE$75)</f>
+        <f t="shared" si="3"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AG7" s="6">
-        <f>SUMPRODUCT(R6:T8,$AC$73:$AE$75)</f>
+        <f t="shared" si="3"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AH7" s="6">
-        <f>SUMPRODUCT(S6:U8,$AC$73:$AE$75)</f>
+        <f t="shared" si="3"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AI7" s="6"/>
@@ -2895,7 +2895,7 @@
         <v>55.000099999999996</v>
       </c>
       <c r="AM7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>325.00109999999995</v>
       </c>
     </row>
@@ -2934,35 +2934,35 @@
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
       <c r="N8" s="6">
-        <f>SUMPRODUCT(B18:D20,$N$79:$P$81) + SUMPRODUCT(B7:D9,$N$73:$P$75) + SUMPRODUCT(B29:D31,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="O8" s="6">
-        <f>SUMPRODUCT(C18:E20,$N$79:$P$81) + SUMPRODUCT(C7:E9,$N$73:$P$75) + SUMPRODUCT(C29:E31,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="P8" s="6">
-        <f>SUMPRODUCT(D18:F20,$N$79:$P$81) + SUMPRODUCT(D7:F9,$N$73:$P$75) + SUMPRODUCT(D29:F31,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="Q8" s="6">
-        <f>SUMPRODUCT(E18:G20,$N$79:$P$81) + SUMPRODUCT(E7:G9,$N$73:$P$75) + SUMPRODUCT(E29:G31,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="R8" s="6">
-        <f>SUMPRODUCT(F18:H20,$N$79:$P$81) + SUMPRODUCT(F7:H9,$N$73:$P$75) + SUMPRODUCT(F29:H31,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="S8" s="6">
-        <f>SUMPRODUCT(G18:I20,$N$79:$P$81) + SUMPRODUCT(G7:I9,$N$73:$P$75) + SUMPRODUCT(G29:I31,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="T8" s="6">
-        <f>SUMPRODUCT(H18:J20,$N$79:$P$81) + SUMPRODUCT(H7:J9,$N$73:$P$75) + SUMPRODUCT(H29:J31,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="U8" s="6">
-        <f>SUMPRODUCT(I18:K20,$N$79:$P$81) + SUMPRODUCT(I7:K9,$N$73:$P$75) + SUMPRODUCT(I29:K31,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="V8" s="6"/>
@@ -2973,33 +2973,33 @@
       <c r="AA8" s="7"/>
       <c r="AB8" s="5"/>
       <c r="AC8" s="6">
-        <f>SUMPRODUCT(N7:P9,$AC$73:$AE$75)</f>
+        <f t="shared" si="3"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AD8" s="6">
-        <f>SUMPRODUCT(O7:Q9,$AC$73:$AE$75)</f>
+        <f t="shared" si="3"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AE8" s="6">
-        <f>SUMPRODUCT(P7:R9,$AC$73:$AE$75)</f>
+        <f t="shared" si="3"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AF8" s="6">
-        <f>SUMPRODUCT(Q7:S9,$AC$73:$AE$75)</f>
+        <f t="shared" si="3"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AG8" s="6">
-        <f>SUMPRODUCT(R7:T9,$AC$73:$AE$75)</f>
+        <f t="shared" si="3"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AH8" s="6">
-        <f>SUMPRODUCT(S7:U9,$AC$73:$AE$75)</f>
+        <f t="shared" si="3"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AI8" s="6"/>
       <c r="AJ8" s="7"/>
       <c r="AL8" s="1">
-        <f t="shared" ref="AL8:AL13" si="2">AD4</f>
+        <f t="shared" ref="AL8:AL13" si="4">AD4</f>
         <v>55.000099999999996</v>
       </c>
       <c r="AM8" s="1">
@@ -3042,35 +3042,35 @@
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
       <c r="N9" s="6">
-        <f>SUMPRODUCT(B19:D21,$N$79:$P$81) + SUMPRODUCT(B8:D10,$N$73:$P$75) + SUMPRODUCT(B30:D32,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="O9" s="6">
-        <f>SUMPRODUCT(C19:E21,$N$79:$P$81) + SUMPRODUCT(C8:E10,$N$73:$P$75) + SUMPRODUCT(C30:E32,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="P9" s="6">
-        <f>SUMPRODUCT(D19:F21,$N$79:$P$81) + SUMPRODUCT(D8:F10,$N$73:$P$75) + SUMPRODUCT(D30:F32,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="Q9" s="6">
-        <f>SUMPRODUCT(E19:G21,$N$79:$P$81) + SUMPRODUCT(E8:G10,$N$73:$P$75) + SUMPRODUCT(E30:G32,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="R9" s="6">
-        <f>SUMPRODUCT(F19:H21,$N$79:$P$81) + SUMPRODUCT(F8:H10,$N$73:$P$75) + SUMPRODUCT(F30:H32,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="S9" s="6">
-        <f>SUMPRODUCT(G19:I21,$N$79:$P$81) + SUMPRODUCT(G8:I10,$N$73:$P$75) + SUMPRODUCT(G30:I32,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="T9" s="6">
-        <f>SUMPRODUCT(H19:J21,$N$79:$P$81) + SUMPRODUCT(H8:J10,$N$73:$P$75) + SUMPRODUCT(H30:J32,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="U9" s="6">
-        <f>SUMPRODUCT(I19:K21,$N$79:$P$81) + SUMPRODUCT(I8:K10,$N$73:$P$75) + SUMPRODUCT(I30:K32,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="V9" s="6"/>
@@ -3081,37 +3081,37 @@
       <c r="AA9" s="7"/>
       <c r="AB9" s="5"/>
       <c r="AC9" s="6">
-        <f>SUMPRODUCT(N8:P10,$AC$73:$AE$75)</f>
+        <f t="shared" si="3"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AD9" s="6">
-        <f>SUMPRODUCT(O8:Q10,$AC$73:$AE$75)</f>
+        <f t="shared" si="3"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AE9" s="6">
-        <f>SUMPRODUCT(P8:R10,$AC$73:$AE$75)</f>
+        <f t="shared" si="3"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AF9" s="6">
-        <f>SUMPRODUCT(Q8:S10,$AC$73:$AE$75)</f>
+        <f t="shared" si="3"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AG9" s="6">
-        <f>SUMPRODUCT(R8:T10,$AC$73:$AE$75)</f>
+        <f t="shared" si="3"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AH9" s="6">
-        <f>SUMPRODUCT(S8:U10,$AC$73:$AE$75)</f>
+        <f t="shared" si="3"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AI9" s="6"/>
       <c r="AJ9" s="7"/>
       <c r="AL9" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AM9" s="1">
-        <f t="shared" ref="AM9:AM13" si="3">AD38</f>
+        <f t="shared" ref="AM9:AM13" si="5">AD38</f>
         <v>325.00109999999995</v>
       </c>
     </row>
@@ -3150,35 +3150,35 @@
       <c r="L10" s="6"/>
       <c r="M10" s="6"/>
       <c r="N10" s="6">
-        <f>SUMPRODUCT(B20:D22,$N$79:$P$81) + SUMPRODUCT(B9:D11,$N$73:$P$75) + SUMPRODUCT(B31:D33,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="O10" s="6">
-        <f>SUMPRODUCT(C20:E22,$N$79:$P$81) + SUMPRODUCT(C9:E11,$N$73:$P$75) + SUMPRODUCT(C31:E33,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="P10" s="6">
-        <f>SUMPRODUCT(D20:F22,$N$79:$P$81) + SUMPRODUCT(D9:F11,$N$73:$P$75) + SUMPRODUCT(D31:F33,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="Q10" s="6">
-        <f>SUMPRODUCT(E20:G22,$N$79:$P$81) + SUMPRODUCT(E9:G11,$N$73:$P$75) + SUMPRODUCT(E31:G33,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="R10" s="6">
-        <f>SUMPRODUCT(F20:H22,$N$79:$P$81) + SUMPRODUCT(F9:H11,$N$73:$P$75) + SUMPRODUCT(F31:H33,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="S10" s="6">
-        <f>SUMPRODUCT(G20:I22,$N$79:$P$81) + SUMPRODUCT(G9:I11,$N$73:$P$75) + SUMPRODUCT(G31:I33,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="T10" s="6">
-        <f>SUMPRODUCT(H20:J22,$N$79:$P$81) + SUMPRODUCT(H9:J11,$N$73:$P$75) + SUMPRODUCT(H31:J33,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="U10" s="6">
-        <f>SUMPRODUCT(I20:K22,$N$79:$P$81) + SUMPRODUCT(I9:K11,$N$73:$P$75) + SUMPRODUCT(I31:K33,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="1"/>
         <v>55.000100000000003</v>
       </c>
       <c r="V10" s="6"/>
@@ -3197,11 +3197,11 @@
       <c r="AI10" s="6"/>
       <c r="AJ10" s="7"/>
       <c r="AL10" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AM10" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>325.00109999999995</v>
       </c>
       <c r="AO10" s="1" t="s">
@@ -3274,11 +3274,11 @@
       <c r="AI11" s="6"/>
       <c r="AJ11" s="7"/>
       <c r="AL11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AM11" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>325.00109999999995</v>
       </c>
       <c r="AP11" s="1">
@@ -3328,11 +3328,11 @@
       <c r="AI12" s="6"/>
       <c r="AJ12" s="7"/>
       <c r="AL12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AM12" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>325.00109999999995</v>
       </c>
     </row>
@@ -3394,11 +3394,11 @@
       <c r="AI13" s="6"/>
       <c r="AJ13" s="7"/>
       <c r="AL13" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AM13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>325.00109999999995</v>
       </c>
     </row>
@@ -3437,35 +3437,35 @@
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
       <c r="N14" s="6">
-        <f>SUMPRODUCT(B13:D15,$U$79:$W$81) + SUMPRODUCT(B2:D4,$U$73:$W$75) + SUMPRODUCT(B24:D26,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" ref="N14:U21" si="6">SUMPRODUCT(B13:D15,$U$79:$W$81) + SUMPRODUCT(B2:D4,$U$73:$W$75) + SUMPRODUCT(B24:D26,$U$85:$W$87) + $Z$73</f>
         <v>55</v>
       </c>
       <c r="O14" s="6">
-        <f>SUMPRODUCT(C13:E15,$U$79:$W$81) + SUMPRODUCT(C2:E4,$U$73:$W$75) + SUMPRODUCT(C24:E26,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="P14" s="6">
-        <f>SUMPRODUCT(D13:F15,$U$79:$W$81) + SUMPRODUCT(D2:F4,$U$73:$W$75) + SUMPRODUCT(D24:F26,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="Q14" s="6">
-        <f>SUMPRODUCT(E13:G15,$U$79:$W$81) + SUMPRODUCT(E2:G4,$U$73:$W$75) + SUMPRODUCT(E24:G26,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="R14" s="6">
-        <f>SUMPRODUCT(F13:H15,$U$79:$W$81) + SUMPRODUCT(F2:H4,$U$73:$W$75) + SUMPRODUCT(F24:H26,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="S14" s="6">
-        <f>SUMPRODUCT(G13:I15,$U$79:$W$81) + SUMPRODUCT(G2:I4,$U$73:$W$75) + SUMPRODUCT(G24:I26,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="T14" s="6">
-        <f>SUMPRODUCT(H13:J15,$U$79:$W$81) + SUMPRODUCT(H2:J4,$U$73:$W$75) + SUMPRODUCT(H24:J26,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="U14" s="6">
-        <f>SUMPRODUCT(I13:K15,$U$79:$W$81) + SUMPRODUCT(I2:K4,$U$73:$W$75) + SUMPRODUCT(I24:K26,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="V14" s="6"/>
@@ -3484,7 +3484,7 @@
       <c r="AI14" s="6"/>
       <c r="AJ14" s="7"/>
       <c r="AL14" s="1">
-        <f t="shared" ref="AL14:AL19" si="4">AE4</f>
+        <f t="shared" ref="AL14:AL19" si="7">AE4</f>
         <v>55.000099999999996</v>
       </c>
       <c r="AM14" s="1">
@@ -3534,35 +3534,35 @@
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
       <c r="N15" s="6">
-        <f>SUMPRODUCT(B14:D16,$U$79:$W$81) + SUMPRODUCT(B3:D5,$U$73:$W$75) + SUMPRODUCT(B25:D27,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="O15" s="6">
-        <f>SUMPRODUCT(C14:E16,$U$79:$W$81) + SUMPRODUCT(C3:E5,$U$73:$W$75) + SUMPRODUCT(C25:E27,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="P15" s="6">
-        <f>SUMPRODUCT(D14:F16,$U$79:$W$81) + SUMPRODUCT(D3:F5,$U$73:$W$75) + SUMPRODUCT(D25:F27,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="Q15" s="6">
-        <f>SUMPRODUCT(E14:G16,$U$79:$W$81) + SUMPRODUCT(E3:G5,$U$73:$W$75) + SUMPRODUCT(E25:G27,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="R15" s="6">
-        <f>SUMPRODUCT(F14:H16,$U$79:$W$81) + SUMPRODUCT(F3:H5,$U$73:$W$75) + SUMPRODUCT(F25:H27,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="S15" s="6">
-        <f>SUMPRODUCT(G14:I16,$U$79:$W$81) + SUMPRODUCT(G3:I5,$U$73:$W$75) + SUMPRODUCT(G25:I27,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="T15" s="6">
-        <f>SUMPRODUCT(H14:J16,$U$79:$W$81) + SUMPRODUCT(H3:J5,$U$73:$W$75) + SUMPRODUCT(H25:J27,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="U15" s="6">
-        <f>SUMPRODUCT(I14:K16,$U$79:$W$81) + SUMPRODUCT(I3:K5,$U$73:$W$75) + SUMPRODUCT(I25:K27,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="V15" s="6"/>
@@ -3573,37 +3573,37 @@
       <c r="AA15" s="7"/>
       <c r="AB15" s="5"/>
       <c r="AC15" s="6">
-        <f>SUMPRODUCT(N14:P16,$AC$73:$AE$75)</f>
+        <f t="shared" ref="AC15:AH20" si="8">SUMPRODUCT(N14:P16,$AC$73:$AE$75)</f>
         <v>55</v>
       </c>
       <c r="AD15" s="6">
-        <f>SUMPRODUCT(O14:Q16,$AC$73:$AE$75)</f>
+        <f t="shared" si="8"/>
         <v>55</v>
       </c>
       <c r="AE15" s="6">
-        <f>SUMPRODUCT(P14:R16,$AC$73:$AE$75)</f>
+        <f t="shared" si="8"/>
         <v>55</v>
       </c>
       <c r="AF15" s="6">
-        <f>SUMPRODUCT(Q14:S16,$AC$73:$AE$75)</f>
+        <f t="shared" si="8"/>
         <v>55</v>
       </c>
       <c r="AG15" s="6">
-        <f>SUMPRODUCT(R14:T16,$AC$73:$AE$75)</f>
+        <f t="shared" si="8"/>
         <v>55</v>
       </c>
       <c r="AH15" s="6">
-        <f>SUMPRODUCT(S14:U16,$AC$73:$AE$75)</f>
+        <f t="shared" si="8"/>
         <v>55</v>
       </c>
       <c r="AI15" s="6"/>
       <c r="AJ15" s="7"/>
       <c r="AL15" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AM15" s="1">
-        <f t="shared" ref="AM15:AM19" si="5">AE38</f>
+        <f t="shared" ref="AM15:AM19" si="9">AE38</f>
         <v>325.00109999999995</v>
       </c>
     </row>
@@ -3642,35 +3642,35 @@
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
       <c r="N16" s="6">
-        <f>SUMPRODUCT(B15:D17,$U$79:$W$81) + SUMPRODUCT(B4:D6,$U$73:$W$75) + SUMPRODUCT(B26:D28,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="O16" s="6">
-        <f>SUMPRODUCT(C15:E17,$U$79:$W$81) + SUMPRODUCT(C4:E6,$U$73:$W$75) + SUMPRODUCT(C26:E28,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="P16" s="6">
-        <f>SUMPRODUCT(D15:F17,$U$79:$W$81) + SUMPRODUCT(D4:F6,$U$73:$W$75) + SUMPRODUCT(D26:F28,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="Q16" s="6">
-        <f>SUMPRODUCT(E15:G17,$U$79:$W$81) + SUMPRODUCT(E4:G6,$U$73:$W$75) + SUMPRODUCT(E26:G28,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="R16" s="6">
-        <f>SUMPRODUCT(F15:H17,$U$79:$W$81) + SUMPRODUCT(F4:H6,$U$73:$W$75) + SUMPRODUCT(F26:H28,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="S16" s="6">
-        <f>SUMPRODUCT(G15:I17,$U$79:$W$81) + SUMPRODUCT(G4:I6,$U$73:$W$75) + SUMPRODUCT(G26:I28,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="T16" s="6">
-        <f>SUMPRODUCT(H15:J17,$U$79:$W$81) + SUMPRODUCT(H4:J6,$U$73:$W$75) + SUMPRODUCT(H26:J28,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="U16" s="6">
-        <f>SUMPRODUCT(I15:K17,$U$79:$W$81) + SUMPRODUCT(I4:K6,$U$73:$W$75) + SUMPRODUCT(I26:K28,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="V16" s="6"/>
@@ -3681,37 +3681,37 @@
       <c r="AA16" s="7"/>
       <c r="AB16" s="5"/>
       <c r="AC16" s="6">
-        <f>SUMPRODUCT(N15:P17,$AC$73:$AE$75)</f>
+        <f t="shared" si="8"/>
         <v>55</v>
       </c>
       <c r="AD16" s="6">
-        <f>SUMPRODUCT(O15:Q17,$AC$73:$AE$75)</f>
+        <f t="shared" si="8"/>
         <v>55</v>
       </c>
       <c r="AE16" s="6">
-        <f>SUMPRODUCT(P15:R17,$AC$73:$AE$75)</f>
+        <f t="shared" si="8"/>
         <v>55</v>
       </c>
       <c r="AF16" s="6">
-        <f>SUMPRODUCT(Q15:S17,$AC$73:$AE$75)</f>
+        <f t="shared" si="8"/>
         <v>55</v>
       </c>
       <c r="AG16" s="6">
-        <f>SUMPRODUCT(R15:T17,$AC$73:$AE$75)</f>
+        <f t="shared" si="8"/>
         <v>55</v>
       </c>
       <c r="AH16" s="6">
-        <f>SUMPRODUCT(S15:U17,$AC$73:$AE$75)</f>
+        <f t="shared" si="8"/>
         <v>55</v>
       </c>
       <c r="AI16" s="6"/>
       <c r="AJ16" s="7"/>
       <c r="AL16" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AM16" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>325.00109999999995</v>
       </c>
       <c r="AO16" s="1" t="s">
@@ -3763,35 +3763,35 @@
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
       <c r="N17" s="6">
-        <f>SUMPRODUCT(B16:D18,$U$79:$W$81) + SUMPRODUCT(B5:D7,$U$73:$W$75) + SUMPRODUCT(B27:D29,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="O17" s="6">
-        <f>SUMPRODUCT(C16:E18,$U$79:$W$81) + SUMPRODUCT(C5:E7,$U$73:$W$75) + SUMPRODUCT(C27:E29,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="P17" s="6">
-        <f>SUMPRODUCT(D16:F18,$U$79:$W$81) + SUMPRODUCT(D5:F7,$U$73:$W$75) + SUMPRODUCT(D27:F29,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="Q17" s="6">
-        <f>SUMPRODUCT(E16:G18,$U$79:$W$81) + SUMPRODUCT(E5:G7,$U$73:$W$75) + SUMPRODUCT(E27:G29,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="R17" s="6">
-        <f>SUMPRODUCT(F16:H18,$U$79:$W$81) + SUMPRODUCT(F5:H7,$U$73:$W$75) + SUMPRODUCT(F27:H29,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="S17" s="6">
-        <f>SUMPRODUCT(G16:I18,$U$79:$W$81) + SUMPRODUCT(G5:I7,$U$73:$W$75) + SUMPRODUCT(G27:I29,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="T17" s="6">
-        <f>SUMPRODUCT(H16:J18,$U$79:$W$81) + SUMPRODUCT(H5:J7,$U$73:$W$75) + SUMPRODUCT(H27:J29,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="U17" s="6">
-        <f>SUMPRODUCT(I16:K18,$U$79:$W$81) + SUMPRODUCT(I5:K7,$U$73:$W$75) + SUMPRODUCT(I27:K29,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="V17" s="6"/>
@@ -3802,37 +3802,37 @@
       <c r="AA17" s="7"/>
       <c r="AB17" s="5"/>
       <c r="AC17" s="6">
-        <f>SUMPRODUCT(N16:P18,$AC$73:$AE$75)</f>
+        <f t="shared" si="8"/>
         <v>55</v>
       </c>
       <c r="AD17" s="6">
-        <f>SUMPRODUCT(O16:Q18,$AC$73:$AE$75)</f>
+        <f t="shared" si="8"/>
         <v>55</v>
       </c>
       <c r="AE17" s="6">
-        <f>SUMPRODUCT(P16:R18,$AC$73:$AE$75)</f>
+        <f t="shared" si="8"/>
         <v>55</v>
       </c>
       <c r="AF17" s="6">
-        <f>SUMPRODUCT(Q16:S18,$AC$73:$AE$75)</f>
+        <f t="shared" si="8"/>
         <v>55</v>
       </c>
       <c r="AG17" s="6">
-        <f>SUMPRODUCT(R16:T18,$AC$73:$AE$75)</f>
+        <f t="shared" si="8"/>
         <v>55</v>
       </c>
       <c r="AH17" s="6">
-        <f>SUMPRODUCT(S16:U18,$AC$73:$AE$75)</f>
+        <f t="shared" si="8"/>
         <v>55</v>
       </c>
       <c r="AI17" s="6"/>
       <c r="AJ17" s="7"/>
       <c r="AL17" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AM17" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>325.00109999999995</v>
       </c>
     </row>
@@ -3871,35 +3871,35 @@
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
       <c r="N18" s="6">
-        <f>SUMPRODUCT(B17:D19,$U$79:$W$81) + SUMPRODUCT(B6:D8,$U$73:$W$75) + SUMPRODUCT(B28:D30,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="O18" s="6">
-        <f>SUMPRODUCT(C17:E19,$U$79:$W$81) + SUMPRODUCT(C6:E8,$U$73:$W$75) + SUMPRODUCT(C28:E30,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="P18" s="6">
-        <f>SUMPRODUCT(D17:F19,$U$79:$W$81) + SUMPRODUCT(D6:F8,$U$73:$W$75) + SUMPRODUCT(D28:F30,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="Q18" s="6">
-        <f>SUMPRODUCT(E17:G19,$U$79:$W$81) + SUMPRODUCT(E6:G8,$U$73:$W$75) + SUMPRODUCT(E28:G30,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="R18" s="6">
-        <f>SUMPRODUCT(F17:H19,$U$79:$W$81) + SUMPRODUCT(F6:H8,$U$73:$W$75) + SUMPRODUCT(F28:H30,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="S18" s="6">
-        <f>SUMPRODUCT(G17:I19,$U$79:$W$81) + SUMPRODUCT(G6:I8,$U$73:$W$75) + SUMPRODUCT(G28:I30,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="T18" s="6">
-        <f>SUMPRODUCT(H17:J19,$U$79:$W$81) + SUMPRODUCT(H6:J8,$U$73:$W$75) + SUMPRODUCT(H28:J30,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="U18" s="6">
-        <f>SUMPRODUCT(I17:K19,$U$79:$W$81) + SUMPRODUCT(I6:K8,$U$73:$W$75) + SUMPRODUCT(I28:K30,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="V18" s="6"/>
@@ -3910,37 +3910,37 @@
       <c r="AA18" s="7"/>
       <c r="AB18" s="5"/>
       <c r="AC18" s="6">
-        <f>SUMPRODUCT(N17:P19,$AC$73:$AE$75)</f>
+        <f t="shared" si="8"/>
         <v>55</v>
       </c>
       <c r="AD18" s="6">
-        <f>SUMPRODUCT(O17:Q19,$AC$73:$AE$75)</f>
+        <f t="shared" si="8"/>
         <v>55</v>
       </c>
       <c r="AE18" s="6">
-        <f>SUMPRODUCT(P17:R19,$AC$73:$AE$75)</f>
+        <f t="shared" si="8"/>
         <v>55</v>
       </c>
       <c r="AF18" s="6">
-        <f>SUMPRODUCT(Q17:S19,$AC$73:$AE$75)</f>
+        <f t="shared" si="8"/>
         <v>55</v>
       </c>
       <c r="AG18" s="6">
-        <f>SUMPRODUCT(R17:T19,$AC$73:$AE$75)</f>
+        <f t="shared" si="8"/>
         <v>55</v>
       </c>
       <c r="AH18" s="6">
-        <f>SUMPRODUCT(S17:U19,$AC$73:$AE$75)</f>
+        <f t="shared" si="8"/>
         <v>55</v>
       </c>
       <c r="AI18" s="6"/>
       <c r="AJ18" s="7"/>
       <c r="AL18" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AM18" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>325.00109999999995</v>
       </c>
     </row>
@@ -3979,35 +3979,35 @@
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
       <c r="N19" s="6">
-        <f>SUMPRODUCT(B18:D20,$U$79:$W$81) + SUMPRODUCT(B7:D9,$U$73:$W$75) + SUMPRODUCT(B29:D31,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="O19" s="6">
-        <f>SUMPRODUCT(C18:E20,$U$79:$W$81) + SUMPRODUCT(C7:E9,$U$73:$W$75) + SUMPRODUCT(C29:E31,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="P19" s="6">
-        <f>SUMPRODUCT(D18:F20,$U$79:$W$81) + SUMPRODUCT(D7:F9,$U$73:$W$75) + SUMPRODUCT(D29:F31,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="Q19" s="6">
-        <f>SUMPRODUCT(E18:G20,$U$79:$W$81) + SUMPRODUCT(E7:G9,$U$73:$W$75) + SUMPRODUCT(E29:G31,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="R19" s="6">
-        <f>SUMPRODUCT(F18:H20,$U$79:$W$81) + SUMPRODUCT(F7:H9,$U$73:$W$75) + SUMPRODUCT(F29:H31,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="S19" s="6">
-        <f>SUMPRODUCT(G18:I20,$U$79:$W$81) + SUMPRODUCT(G7:I9,$U$73:$W$75) + SUMPRODUCT(G29:I31,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="T19" s="6">
-        <f>SUMPRODUCT(H18:J20,$U$79:$W$81) + SUMPRODUCT(H7:J9,$U$73:$W$75) + SUMPRODUCT(H29:J31,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="U19" s="6">
-        <f>SUMPRODUCT(I18:K20,$U$79:$W$81) + SUMPRODUCT(I7:K9,$U$73:$W$75) + SUMPRODUCT(I29:K31,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="V19" s="6"/>
@@ -4018,37 +4018,37 @@
       <c r="AA19" s="7"/>
       <c r="AB19" s="5"/>
       <c r="AC19" s="6">
-        <f>SUMPRODUCT(N18:P20,$AC$73:$AE$75)</f>
+        <f t="shared" si="8"/>
         <v>55</v>
       </c>
       <c r="AD19" s="6">
-        <f>SUMPRODUCT(O18:Q20,$AC$73:$AE$75)</f>
+        <f t="shared" si="8"/>
         <v>55</v>
       </c>
       <c r="AE19" s="6">
-        <f>SUMPRODUCT(P18:R20,$AC$73:$AE$75)</f>
+        <f t="shared" si="8"/>
         <v>55</v>
       </c>
       <c r="AF19" s="6">
-        <f>SUMPRODUCT(Q18:S20,$AC$73:$AE$75)</f>
+        <f t="shared" si="8"/>
         <v>55</v>
       </c>
       <c r="AG19" s="6">
-        <f>SUMPRODUCT(R18:T20,$AC$73:$AE$75)</f>
+        <f t="shared" si="8"/>
         <v>55</v>
       </c>
       <c r="AH19" s="6">
-        <f>SUMPRODUCT(S18:U20,$AC$73:$AE$75)</f>
+        <f t="shared" si="8"/>
         <v>55</v>
       </c>
       <c r="AI19" s="6"/>
       <c r="AJ19" s="7"/>
       <c r="AL19" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AM19" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>325.00109999999995</v>
       </c>
     </row>
@@ -4087,35 +4087,35 @@
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
       <c r="N20" s="6">
-        <f>SUMPRODUCT(B19:D21,$U$79:$W$81) + SUMPRODUCT(B8:D10,$U$73:$W$75) + SUMPRODUCT(B30:D32,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="O20" s="6">
-        <f>SUMPRODUCT(C19:E21,$U$79:$W$81) + SUMPRODUCT(C8:E10,$U$73:$W$75) + SUMPRODUCT(C30:E32,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="P20" s="6">
-        <f>SUMPRODUCT(D19:F21,$U$79:$W$81) + SUMPRODUCT(D8:F10,$U$73:$W$75) + SUMPRODUCT(D30:F32,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="Q20" s="6">
-        <f>SUMPRODUCT(E19:G21,$U$79:$W$81) + SUMPRODUCT(E8:G10,$U$73:$W$75) + SUMPRODUCT(E30:G32,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="R20" s="6">
-        <f>SUMPRODUCT(F19:H21,$U$79:$W$81) + SUMPRODUCT(F8:H10,$U$73:$W$75) + SUMPRODUCT(F30:H32,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="S20" s="6">
-        <f>SUMPRODUCT(G19:I21,$U$79:$W$81) + SUMPRODUCT(G8:I10,$U$73:$W$75) + SUMPRODUCT(G30:I32,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="T20" s="6">
-        <f>SUMPRODUCT(H19:J21,$U$79:$W$81) + SUMPRODUCT(H8:J10,$U$73:$W$75) + SUMPRODUCT(H30:J32,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="U20" s="6">
-        <f>SUMPRODUCT(I19:K21,$U$79:$W$81) + SUMPRODUCT(I8:K10,$U$73:$W$75) + SUMPRODUCT(I30:K32,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="V20" s="6"/>
@@ -4126,33 +4126,33 @@
       <c r="AA20" s="7"/>
       <c r="AB20" s="5"/>
       <c r="AC20" s="6">
-        <f>SUMPRODUCT(N19:P21,$AC$73:$AE$75)</f>
+        <f t="shared" si="8"/>
         <v>55</v>
       </c>
       <c r="AD20" s="6">
-        <f>SUMPRODUCT(O19:Q21,$AC$73:$AE$75)</f>
+        <f t="shared" si="8"/>
         <v>55</v>
       </c>
       <c r="AE20" s="6">
-        <f>SUMPRODUCT(P19:R21,$AC$73:$AE$75)</f>
+        <f t="shared" si="8"/>
         <v>55</v>
       </c>
       <c r="AF20" s="6">
-        <f>SUMPRODUCT(Q19:S21,$AC$73:$AE$75)</f>
+        <f t="shared" si="8"/>
         <v>55</v>
       </c>
       <c r="AG20" s="6">
-        <f>SUMPRODUCT(R19:T21,$AC$73:$AE$75)</f>
+        <f t="shared" si="8"/>
         <v>55</v>
       </c>
       <c r="AH20" s="6">
-        <f>SUMPRODUCT(S19:U21,$AC$73:$AE$75)</f>
+        <f t="shared" si="8"/>
         <v>55</v>
       </c>
       <c r="AI20" s="6"/>
       <c r="AJ20" s="7"/>
       <c r="AL20" s="1">
-        <f t="shared" ref="AL20:AL25" si="6">AF4</f>
+        <f t="shared" ref="AL20:AL25" si="10">AF4</f>
         <v>55.000099999999996</v>
       </c>
       <c r="AM20" s="1">
@@ -4195,35 +4195,35 @@
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
       <c r="N21" s="6">
-        <f>SUMPRODUCT(B20:D22,$U$79:$W$81) + SUMPRODUCT(B9:D11,$U$73:$W$75) + SUMPRODUCT(B31:D33,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="O21" s="6">
-        <f>SUMPRODUCT(C20:E22,$U$79:$W$81) + SUMPRODUCT(C9:E11,$U$73:$W$75) + SUMPRODUCT(C31:E33,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="P21" s="6">
-        <f>SUMPRODUCT(D20:F22,$U$79:$W$81) + SUMPRODUCT(D9:F11,$U$73:$W$75) + SUMPRODUCT(D31:F33,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="Q21" s="6">
-        <f>SUMPRODUCT(E20:G22,$U$79:$W$81) + SUMPRODUCT(E9:G11,$U$73:$W$75) + SUMPRODUCT(E31:G33,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="R21" s="6">
-        <f>SUMPRODUCT(F20:H22,$U$79:$W$81) + SUMPRODUCT(F9:H11,$U$73:$W$75) + SUMPRODUCT(F31:H33,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="S21" s="6">
-        <f>SUMPRODUCT(G20:I22,$U$79:$W$81) + SUMPRODUCT(G9:I11,$U$73:$W$75) + SUMPRODUCT(G31:I33,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="T21" s="6">
-        <f>SUMPRODUCT(H20:J22,$U$79:$W$81) + SUMPRODUCT(H9:J11,$U$73:$W$75) + SUMPRODUCT(H31:J33,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="U21" s="6">
-        <f>SUMPRODUCT(I20:K22,$U$79:$W$81) + SUMPRODUCT(I9:K11,$U$73:$W$75) + SUMPRODUCT(I31:K33,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="V21" s="6"/>
@@ -4242,11 +4242,11 @@
       <c r="AI21" s="6"/>
       <c r="AJ21" s="7"/>
       <c r="AL21" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AM21" s="1">
-        <f t="shared" ref="AM21:AM25" si="7">AF38</f>
+        <f t="shared" ref="AM21:AM25" si="11">AF38</f>
         <v>325.00109999999995</v>
       </c>
     </row>
@@ -4308,11 +4308,11 @@
       <c r="AI22" s="6"/>
       <c r="AJ22" s="7"/>
       <c r="AL22" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AM22" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>325.00109999999995</v>
       </c>
     </row>
@@ -4354,11 +4354,11 @@
       <c r="AI23" s="6"/>
       <c r="AJ23" s="7"/>
       <c r="AL23" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AM23" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>325.00109999999995</v>
       </c>
     </row>
@@ -4420,11 +4420,11 @@
       <c r="AI24" s="6"/>
       <c r="AJ24" s="7"/>
       <c r="AL24" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AM24" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>325.00109999999995</v>
       </c>
     </row>
@@ -4486,11 +4486,11 @@
       <c r="AI25" s="6"/>
       <c r="AJ25" s="7"/>
       <c r="AL25" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AM25" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>325.00109999999995</v>
       </c>
     </row>
@@ -4552,7 +4552,7 @@
       <c r="AI26" s="6"/>
       <c r="AJ26" s="7"/>
       <c r="AL26" s="1">
-        <f t="shared" ref="AL26:AL31" si="8">AG4</f>
+        <f t="shared" ref="AL26:AL31" si="12">AG4</f>
         <v>55.000099999999996</v>
       </c>
       <c r="AM26" s="1">
@@ -4618,11 +4618,11 @@
       <c r="AI27" s="6"/>
       <c r="AJ27" s="7"/>
       <c r="AL27" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AM27" s="1">
-        <f t="shared" ref="AM27:AM31" si="9">AG38</f>
+        <f t="shared" ref="AM27:AM31" si="13">AG38</f>
         <v>325.00109999999995</v>
       </c>
     </row>
@@ -4684,11 +4684,11 @@
       <c r="AI28" s="6"/>
       <c r="AJ28" s="7"/>
       <c r="AL28" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AM28" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>325.00109999999995</v>
       </c>
     </row>
@@ -4750,11 +4750,11 @@
       <c r="AI29" s="6"/>
       <c r="AJ29" s="7"/>
       <c r="AL29" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AM29" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>325.00109999999995</v>
       </c>
     </row>
@@ -4816,11 +4816,11 @@
       <c r="AI30" s="6"/>
       <c r="AJ30" s="7"/>
       <c r="AL30" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AM30" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>325.00109999999995</v>
       </c>
     </row>
@@ -4882,11 +4882,11 @@
       <c r="AI31" s="6"/>
       <c r="AJ31" s="7"/>
       <c r="AL31" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AM31" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>325.00109999999995</v>
       </c>
     </row>
@@ -4948,7 +4948,7 @@
       <c r="AI32" s="6"/>
       <c r="AJ32" s="7"/>
       <c r="AL32" s="1">
-        <f t="shared" ref="AL32:AL37" si="10">AH4</f>
+        <f t="shared" ref="AL32:AL37" si="14">AH4</f>
         <v>55.000099999999996</v>
       </c>
       <c r="AM32" s="1">
@@ -5014,11 +5014,11 @@
       <c r="AI33" s="6"/>
       <c r="AJ33" s="7"/>
       <c r="AL33" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AM33" s="1">
-        <f t="shared" ref="AM33:AM37" si="11">AH38</f>
+        <f t="shared" ref="AM33:AM37" si="15">AH38</f>
         <v>325.00109999999995</v>
       </c>
     </row>
@@ -5060,11 +5060,11 @@
       <c r="AI34" s="6"/>
       <c r="AJ34" s="7"/>
       <c r="AL34" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AM34" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>325.00109999999995</v>
       </c>
     </row>
@@ -5126,11 +5126,11 @@
       <c r="AI35" s="6"/>
       <c r="AJ35" s="7"/>
       <c r="AL35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AM35" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>325.00109999999995</v>
       </c>
     </row>
@@ -5169,35 +5169,35 @@
       <c r="L36" s="6"/>
       <c r="M36" s="6"/>
       <c r="N36" s="6">
-        <f>SUMPRODUCT(B46:D48,$N$79:$P$81) + SUMPRODUCT(B35:D37,$N$73:$P$75) + SUMPRODUCT(B57:D59,$N$85:$P$87) + $S$73</f>
+        <f t="shared" ref="N36:U43" si="16">SUMPRODUCT(B46:D48,$N$79:$P$81) + SUMPRODUCT(B35:D37,$N$73:$P$75) + SUMPRODUCT(B57:D59,$N$85:$P$87) + $S$73</f>
         <v>325.00110000000001</v>
       </c>
       <c r="O36" s="6">
-        <f>SUMPRODUCT(C46:E48,$N$79:$P$81) + SUMPRODUCT(C35:E37,$N$73:$P$75) + SUMPRODUCT(C57:E59,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="P36" s="6">
-        <f>SUMPRODUCT(D46:F48,$N$79:$P$81) + SUMPRODUCT(D35:F37,$N$73:$P$75) + SUMPRODUCT(D57:F59,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="Q36" s="6">
-        <f>SUMPRODUCT(E46:G48,$N$79:$P$81) + SUMPRODUCT(E35:G37,$N$73:$P$75) + SUMPRODUCT(E57:G59,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="R36" s="6">
-        <f>SUMPRODUCT(F46:H48,$N$79:$P$81) + SUMPRODUCT(F35:H37,$N$73:$P$75) + SUMPRODUCT(F57:H59,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="S36" s="6">
-        <f>SUMPRODUCT(G46:I48,$N$79:$P$81) + SUMPRODUCT(G35:I37,$N$73:$P$75) + SUMPRODUCT(G57:I59,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="T36" s="6">
-        <f>SUMPRODUCT(H46:J48,$N$79:$P$81) + SUMPRODUCT(H35:J37,$N$73:$P$75) + SUMPRODUCT(H57:J59,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="U36" s="6">
-        <f>SUMPRODUCT(I46:K48,$N$79:$P$81) + SUMPRODUCT(I35:K37,$N$73:$P$75) + SUMPRODUCT(I57:K59,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="V36" s="6"/>
@@ -5216,11 +5216,11 @@
       <c r="AI36" s="6"/>
       <c r="AJ36" s="7"/>
       <c r="AL36" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AM36" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>325.00109999999995</v>
       </c>
     </row>
@@ -5259,35 +5259,35 @@
       <c r="L37" s="6"/>
       <c r="M37" s="6"/>
       <c r="N37" s="6">
-        <f>SUMPRODUCT(B47:D49,$N$79:$P$81) + SUMPRODUCT(B36:D38,$N$73:$P$75) + SUMPRODUCT(B58:D60,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="O37" s="6">
-        <f>SUMPRODUCT(C47:E49,$N$79:$P$81) + SUMPRODUCT(C36:E38,$N$73:$P$75) + SUMPRODUCT(C58:E60,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="P37" s="6">
-        <f>SUMPRODUCT(D47:F49,$N$79:$P$81) + SUMPRODUCT(D36:F38,$N$73:$P$75) + SUMPRODUCT(D58:F60,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="Q37" s="6">
-        <f>SUMPRODUCT(E47:G49,$N$79:$P$81) + SUMPRODUCT(E36:G38,$N$73:$P$75) + SUMPRODUCT(E58:G60,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="R37" s="6">
-        <f>SUMPRODUCT(F47:H49,$N$79:$P$81) + SUMPRODUCT(F36:H38,$N$73:$P$75) + SUMPRODUCT(F58:H60,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="S37" s="6">
-        <f>SUMPRODUCT(G47:I49,$N$79:$P$81) + SUMPRODUCT(G36:I38,$N$73:$P$75) + SUMPRODUCT(G58:I60,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="T37" s="6">
-        <f>SUMPRODUCT(H47:J49,$N$79:$P$81) + SUMPRODUCT(H36:J38,$N$73:$P$75) + SUMPRODUCT(H58:J60,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="U37" s="6">
-        <f>SUMPRODUCT(I47:K49,$N$79:$P$81) + SUMPRODUCT(I36:K38,$N$73:$P$75) + SUMPRODUCT(I58:K60,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="V37" s="6"/>
@@ -5298,37 +5298,37 @@
       <c r="AA37" s="7"/>
       <c r="AB37" s="5"/>
       <c r="AC37" s="6">
-        <f>SUMPRODUCT(N36:P38,$AC$73:$AE$75)</f>
+        <f t="shared" ref="AC37:AH42" si="17">SUMPRODUCT(N36:P38,$AC$73:$AE$75)</f>
         <v>325.00109999999995</v>
       </c>
       <c r="AD37" s="6">
-        <f>SUMPRODUCT(O36:Q38,$AC$73:$AE$75)</f>
+        <f t="shared" si="17"/>
         <v>325.00109999999995</v>
       </c>
       <c r="AE37" s="6">
-        <f>SUMPRODUCT(P36:R38,$AC$73:$AE$75)</f>
+        <f t="shared" si="17"/>
         <v>325.00109999999995</v>
       </c>
       <c r="AF37" s="6">
-        <f>SUMPRODUCT(Q36:S38,$AC$73:$AE$75)</f>
+        <f t="shared" si="17"/>
         <v>325.00109999999995</v>
       </c>
       <c r="AG37" s="6">
-        <f>SUMPRODUCT(R36:T38,$AC$73:$AE$75)</f>
+        <f t="shared" si="17"/>
         <v>325.00109999999995</v>
       </c>
       <c r="AH37" s="6">
-        <f>SUMPRODUCT(S36:U38,$AC$73:$AE$75)</f>
+        <f t="shared" si="17"/>
         <v>325.00109999999995</v>
       </c>
       <c r="AI37" s="6"/>
       <c r="AJ37" s="7"/>
       <c r="AL37" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>55.000099999999996</v>
       </c>
       <c r="AM37" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>325.00109999999995</v>
       </c>
     </row>
@@ -5367,35 +5367,35 @@
       <c r="L38" s="6"/>
       <c r="M38" s="6"/>
       <c r="N38" s="6">
-        <f>SUMPRODUCT(B48:D50,$N$79:$P$81) + SUMPRODUCT(B37:D39,$N$73:$P$75) + SUMPRODUCT(B59:D61,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="O38" s="6">
-        <f>SUMPRODUCT(C48:E50,$N$79:$P$81) + SUMPRODUCT(C37:E39,$N$73:$P$75) + SUMPRODUCT(C59:E61,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="P38" s="6">
-        <f>SUMPRODUCT(D48:F50,$N$79:$P$81) + SUMPRODUCT(D37:F39,$N$73:$P$75) + SUMPRODUCT(D59:F61,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="Q38" s="6">
-        <f>SUMPRODUCT(E48:G50,$N$79:$P$81) + SUMPRODUCT(E37:G39,$N$73:$P$75) + SUMPRODUCT(E59:G61,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="R38" s="6">
-        <f>SUMPRODUCT(F48:H50,$N$79:$P$81) + SUMPRODUCT(F37:H39,$N$73:$P$75) + SUMPRODUCT(F59:H61,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="S38" s="6">
-        <f>SUMPRODUCT(G48:I50,$N$79:$P$81) + SUMPRODUCT(G37:I39,$N$73:$P$75) + SUMPRODUCT(G59:I61,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="T38" s="6">
-        <f>SUMPRODUCT(H48:J50,$N$79:$P$81) + SUMPRODUCT(H37:J39,$N$73:$P$75) + SUMPRODUCT(H59:J61,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="U38" s="6">
-        <f>SUMPRODUCT(I48:K50,$N$79:$P$81) + SUMPRODUCT(I37:K39,$N$73:$P$75) + SUMPRODUCT(I59:K61,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="V38" s="6"/>
@@ -5406,27 +5406,27 @@
       <c r="AA38" s="7"/>
       <c r="AB38" s="5"/>
       <c r="AC38" s="6">
-        <f>SUMPRODUCT(N37:P39,$AC$73:$AE$75)</f>
+        <f t="shared" si="17"/>
         <v>325.00109999999995</v>
       </c>
       <c r="AD38" s="6">
-        <f>SUMPRODUCT(O37:Q39,$AC$73:$AE$75)</f>
+        <f t="shared" si="17"/>
         <v>325.00109999999995</v>
       </c>
       <c r="AE38" s="6">
-        <f>SUMPRODUCT(P37:R39,$AC$73:$AE$75)</f>
+        <f t="shared" si="17"/>
         <v>325.00109999999995</v>
       </c>
       <c r="AF38" s="6">
-        <f>SUMPRODUCT(Q37:S39,$AC$73:$AE$75)</f>
+        <f t="shared" si="17"/>
         <v>325.00109999999995</v>
       </c>
       <c r="AG38" s="6">
-        <f>SUMPRODUCT(R37:T39,$AC$73:$AE$75)</f>
+        <f t="shared" si="17"/>
         <v>325.00109999999995</v>
       </c>
       <c r="AH38" s="6">
-        <f>SUMPRODUCT(S37:U39,$AC$73:$AE$75)</f>
+        <f t="shared" si="17"/>
         <v>325.00109999999995</v>
       </c>
       <c r="AI38" s="6"/>
@@ -5475,35 +5475,35 @@
       <c r="L39" s="6"/>
       <c r="M39" s="6"/>
       <c r="N39" s="6">
-        <f>SUMPRODUCT(B49:D51,$N$79:$P$81) + SUMPRODUCT(B38:D40,$N$73:$P$75) + SUMPRODUCT(B60:D62,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="O39" s="6">
-        <f>SUMPRODUCT(C49:E51,$N$79:$P$81) + SUMPRODUCT(C38:E40,$N$73:$P$75) + SUMPRODUCT(C60:E62,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="P39" s="6">
-        <f>SUMPRODUCT(D49:F51,$N$79:$P$81) + SUMPRODUCT(D38:F40,$N$73:$P$75) + SUMPRODUCT(D60:F62,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="Q39" s="6">
-        <f>SUMPRODUCT(E49:G51,$N$79:$P$81) + SUMPRODUCT(E38:G40,$N$73:$P$75) + SUMPRODUCT(E60:G62,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="R39" s="6">
-        <f>SUMPRODUCT(F49:H51,$N$79:$P$81) + SUMPRODUCT(F38:H40,$N$73:$P$75) + SUMPRODUCT(F60:H62,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="S39" s="6">
-        <f>SUMPRODUCT(G49:I51,$N$79:$P$81) + SUMPRODUCT(G38:I40,$N$73:$P$75) + SUMPRODUCT(G60:I62,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="T39" s="6">
-        <f>SUMPRODUCT(H49:J51,$N$79:$P$81) + SUMPRODUCT(H38:J40,$N$73:$P$75) + SUMPRODUCT(H60:J62,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="U39" s="6">
-        <f>SUMPRODUCT(I49:K51,$N$79:$P$81) + SUMPRODUCT(I38:K40,$N$73:$P$75) + SUMPRODUCT(I60:K62,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="V39" s="6"/>
@@ -5514,37 +5514,37 @@
       <c r="AA39" s="7"/>
       <c r="AB39" s="5"/>
       <c r="AC39" s="6">
-        <f>SUMPRODUCT(N38:P40,$AC$73:$AE$75)</f>
+        <f t="shared" si="17"/>
         <v>325.00109999999995</v>
       </c>
       <c r="AD39" s="6">
-        <f>SUMPRODUCT(O38:Q40,$AC$73:$AE$75)</f>
+        <f t="shared" si="17"/>
         <v>325.00109999999995</v>
       </c>
       <c r="AE39" s="6">
-        <f>SUMPRODUCT(P38:R40,$AC$73:$AE$75)</f>
+        <f t="shared" si="17"/>
         <v>325.00109999999995</v>
       </c>
       <c r="AF39" s="6">
-        <f>SUMPRODUCT(Q38:S40,$AC$73:$AE$75)</f>
+        <f t="shared" si="17"/>
         <v>325.00109999999995</v>
       </c>
       <c r="AG39" s="6">
-        <f>SUMPRODUCT(R38:T40,$AC$73:$AE$75)</f>
+        <f t="shared" si="17"/>
         <v>325.00109999999995</v>
       </c>
       <c r="AH39" s="6">
-        <f>SUMPRODUCT(S38:U40,$AC$73:$AE$75)</f>
+        <f t="shared" si="17"/>
         <v>325.00109999999995</v>
       </c>
       <c r="AI39" s="6"/>
       <c r="AJ39" s="7"/>
       <c r="AL39" s="1">
-        <f t="shared" ref="AL39:AL43" si="12">AC16</f>
+        <f t="shared" ref="AL39:AL43" si="18">AC16</f>
         <v>55</v>
       </c>
       <c r="AM39" s="1">
-        <f t="shared" ref="AM39:AM43" si="13">AC49</f>
+        <f t="shared" ref="AM39:AM43" si="19">AC49</f>
         <v>324.99999999999994</v>
       </c>
     </row>
@@ -5583,35 +5583,35 @@
       <c r="L40" s="6"/>
       <c r="M40" s="6"/>
       <c r="N40" s="6">
-        <f>SUMPRODUCT(B50:D52,$N$79:$P$81) + SUMPRODUCT(B39:D41,$N$73:$P$75) + SUMPRODUCT(B61:D63,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="O40" s="6">
-        <f>SUMPRODUCT(C50:E52,$N$79:$P$81) + SUMPRODUCT(C39:E41,$N$73:$P$75) + SUMPRODUCT(C61:E63,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="P40" s="6">
-        <f>SUMPRODUCT(D50:F52,$N$79:$P$81) + SUMPRODUCT(D39:F41,$N$73:$P$75) + SUMPRODUCT(D61:F63,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="Q40" s="6">
-        <f>SUMPRODUCT(E50:G52,$N$79:$P$81) + SUMPRODUCT(E39:G41,$N$73:$P$75) + SUMPRODUCT(E61:G63,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="R40" s="6">
-        <f>SUMPRODUCT(F50:H52,$N$79:$P$81) + SUMPRODUCT(F39:H41,$N$73:$P$75) + SUMPRODUCT(F61:H63,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="S40" s="6">
-        <f>SUMPRODUCT(G50:I52,$N$79:$P$81) + SUMPRODUCT(G39:I41,$N$73:$P$75) + SUMPRODUCT(G61:I63,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="T40" s="6">
-        <f>SUMPRODUCT(H50:J52,$N$79:$P$81) + SUMPRODUCT(H39:J41,$N$73:$P$75) + SUMPRODUCT(H61:J63,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="U40" s="6">
-        <f>SUMPRODUCT(I50:K52,$N$79:$P$81) + SUMPRODUCT(I39:K41,$N$73:$P$75) + SUMPRODUCT(I61:K63,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="V40" s="6"/>
@@ -5622,37 +5622,37 @@
       <c r="AA40" s="7"/>
       <c r="AB40" s="5"/>
       <c r="AC40" s="6">
-        <f>SUMPRODUCT(N39:P41,$AC$73:$AE$75)</f>
+        <f t="shared" si="17"/>
         <v>325.00109999999995</v>
       </c>
       <c r="AD40" s="6">
-        <f>SUMPRODUCT(O39:Q41,$AC$73:$AE$75)</f>
+        <f t="shared" si="17"/>
         <v>325.00109999999995</v>
       </c>
       <c r="AE40" s="6">
-        <f>SUMPRODUCT(P39:R41,$AC$73:$AE$75)</f>
+        <f t="shared" si="17"/>
         <v>325.00109999999995</v>
       </c>
       <c r="AF40" s="6">
-        <f>SUMPRODUCT(Q39:S41,$AC$73:$AE$75)</f>
+        <f t="shared" si="17"/>
         <v>325.00109999999995</v>
       </c>
       <c r="AG40" s="6">
-        <f>SUMPRODUCT(R39:T41,$AC$73:$AE$75)</f>
+        <f t="shared" si="17"/>
         <v>325.00109999999995</v>
       </c>
       <c r="AH40" s="6">
-        <f>SUMPRODUCT(S39:U41,$AC$73:$AE$75)</f>
+        <f t="shared" si="17"/>
         <v>325.00109999999995</v>
       </c>
       <c r="AI40" s="6"/>
       <c r="AJ40" s="7"/>
       <c r="AL40" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>55</v>
       </c>
       <c r="AM40" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>324.99999999999994</v>
       </c>
     </row>
@@ -5691,35 +5691,35 @@
       <c r="L41" s="6"/>
       <c r="M41" s="6"/>
       <c r="N41" s="6">
-        <f>SUMPRODUCT(B51:D53,$N$79:$P$81) + SUMPRODUCT(B40:D42,$N$73:$P$75) + SUMPRODUCT(B62:D64,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="O41" s="6">
-        <f>SUMPRODUCT(C51:E53,$N$79:$P$81) + SUMPRODUCT(C40:E42,$N$73:$P$75) + SUMPRODUCT(C62:E64,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="P41" s="6">
-        <f>SUMPRODUCT(D51:F53,$N$79:$P$81) + SUMPRODUCT(D40:F42,$N$73:$P$75) + SUMPRODUCT(D62:F64,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="Q41" s="6">
-        <f>SUMPRODUCT(E51:G53,$N$79:$P$81) + SUMPRODUCT(E40:G42,$N$73:$P$75) + SUMPRODUCT(E62:G64,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="R41" s="6">
-        <f>SUMPRODUCT(F51:H53,$N$79:$P$81) + SUMPRODUCT(F40:H42,$N$73:$P$75) + SUMPRODUCT(F62:H64,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="S41" s="6">
-        <f>SUMPRODUCT(G51:I53,$N$79:$P$81) + SUMPRODUCT(G40:I42,$N$73:$P$75) + SUMPRODUCT(G62:I64,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="T41" s="6">
-        <f>SUMPRODUCT(H51:J53,$N$79:$P$81) + SUMPRODUCT(H40:J42,$N$73:$P$75) + SUMPRODUCT(H62:J64,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="U41" s="6">
-        <f>SUMPRODUCT(I51:K53,$N$79:$P$81) + SUMPRODUCT(I40:K42,$N$73:$P$75) + SUMPRODUCT(I62:K64,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="V41" s="6"/>
@@ -5730,37 +5730,37 @@
       <c r="AA41" s="7"/>
       <c r="AB41" s="5"/>
       <c r="AC41" s="6">
-        <f>SUMPRODUCT(N40:P42,$AC$73:$AE$75)</f>
+        <f t="shared" si="17"/>
         <v>325.00109999999995</v>
       </c>
       <c r="AD41" s="6">
-        <f>SUMPRODUCT(O40:Q42,$AC$73:$AE$75)</f>
+        <f t="shared" si="17"/>
         <v>325.00109999999995</v>
       </c>
       <c r="AE41" s="6">
-        <f>SUMPRODUCT(P40:R42,$AC$73:$AE$75)</f>
+        <f t="shared" si="17"/>
         <v>325.00109999999995</v>
       </c>
       <c r="AF41" s="6">
-        <f>SUMPRODUCT(Q40:S42,$AC$73:$AE$75)</f>
+        <f t="shared" si="17"/>
         <v>325.00109999999995</v>
       </c>
       <c r="AG41" s="6">
-        <f>SUMPRODUCT(R40:T42,$AC$73:$AE$75)</f>
+        <f t="shared" si="17"/>
         <v>325.00109999999995</v>
       </c>
       <c r="AH41" s="6">
-        <f>SUMPRODUCT(S40:U42,$AC$73:$AE$75)</f>
+        <f t="shared" si="17"/>
         <v>325.00109999999995</v>
       </c>
       <c r="AI41" s="6"/>
       <c r="AJ41" s="7"/>
       <c r="AL41" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>55</v>
       </c>
       <c r="AM41" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>324.99999999999994</v>
       </c>
     </row>
@@ -5799,35 +5799,35 @@
       <c r="L42" s="6"/>
       <c r="M42" s="6"/>
       <c r="N42" s="6">
-        <f>SUMPRODUCT(B52:D54,$N$79:$P$81) + SUMPRODUCT(B41:D43,$N$73:$P$75) + SUMPRODUCT(B63:D65,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="O42" s="6">
-        <f>SUMPRODUCT(C52:E54,$N$79:$P$81) + SUMPRODUCT(C41:E43,$N$73:$P$75) + SUMPRODUCT(C63:E65,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="P42" s="6">
-        <f>SUMPRODUCT(D52:F54,$N$79:$P$81) + SUMPRODUCT(D41:F43,$N$73:$P$75) + SUMPRODUCT(D63:F65,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="Q42" s="6">
-        <f>SUMPRODUCT(E52:G54,$N$79:$P$81) + SUMPRODUCT(E41:G43,$N$73:$P$75) + SUMPRODUCT(E63:G65,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="R42" s="6">
-        <f>SUMPRODUCT(F52:H54,$N$79:$P$81) + SUMPRODUCT(F41:H43,$N$73:$P$75) + SUMPRODUCT(F63:H65,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="S42" s="6">
-        <f>SUMPRODUCT(G52:I54,$N$79:$P$81) + SUMPRODUCT(G41:I43,$N$73:$P$75) + SUMPRODUCT(G63:I65,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="T42" s="6">
-        <f>SUMPRODUCT(H52:J54,$N$79:$P$81) + SUMPRODUCT(H41:J43,$N$73:$P$75) + SUMPRODUCT(H63:J65,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="U42" s="6">
-        <f>SUMPRODUCT(I52:K54,$N$79:$P$81) + SUMPRODUCT(I41:K43,$N$73:$P$75) + SUMPRODUCT(I63:K65,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="V42" s="6"/>
@@ -5838,37 +5838,37 @@
       <c r="AA42" s="7"/>
       <c r="AB42" s="5"/>
       <c r="AC42" s="6">
-        <f>SUMPRODUCT(N41:P43,$AC$73:$AE$75)</f>
+        <f t="shared" si="17"/>
         <v>325.00109999999995</v>
       </c>
       <c r="AD42" s="6">
-        <f>SUMPRODUCT(O41:Q43,$AC$73:$AE$75)</f>
+        <f t="shared" si="17"/>
         <v>325.00109999999995</v>
       </c>
       <c r="AE42" s="6">
-        <f>SUMPRODUCT(P41:R43,$AC$73:$AE$75)</f>
+        <f t="shared" si="17"/>
         <v>325.00109999999995</v>
       </c>
       <c r="AF42" s="6">
-        <f>SUMPRODUCT(Q41:S43,$AC$73:$AE$75)</f>
+        <f t="shared" si="17"/>
         <v>325.00109999999995</v>
       </c>
       <c r="AG42" s="6">
-        <f>SUMPRODUCT(R41:T43,$AC$73:$AE$75)</f>
+        <f t="shared" si="17"/>
         <v>325.00109999999995</v>
       </c>
       <c r="AH42" s="6">
-        <f>SUMPRODUCT(S41:U43,$AC$73:$AE$75)</f>
+        <f t="shared" si="17"/>
         <v>325.00109999999995</v>
       </c>
       <c r="AI42" s="6"/>
       <c r="AJ42" s="7"/>
       <c r="AL42" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>55</v>
       </c>
       <c r="AM42" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>324.99999999999994</v>
       </c>
     </row>
@@ -5907,35 +5907,35 @@
       <c r="L43" s="6"/>
       <c r="M43" s="6"/>
       <c r="N43" s="6">
-        <f>SUMPRODUCT(B53:D55,$N$79:$P$81) + SUMPRODUCT(B42:D44,$N$73:$P$75) + SUMPRODUCT(B64:D66,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="O43" s="6">
-        <f>SUMPRODUCT(C53:E55,$N$79:$P$81) + SUMPRODUCT(C42:E44,$N$73:$P$75) + SUMPRODUCT(C64:E66,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="P43" s="6">
-        <f>SUMPRODUCT(D53:F55,$N$79:$P$81) + SUMPRODUCT(D42:F44,$N$73:$P$75) + SUMPRODUCT(D64:F66,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="Q43" s="6">
-        <f>SUMPRODUCT(E53:G55,$N$79:$P$81) + SUMPRODUCT(E42:G44,$N$73:$P$75) + SUMPRODUCT(E64:G66,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="R43" s="6">
-        <f>SUMPRODUCT(F53:H55,$N$79:$P$81) + SUMPRODUCT(F42:H44,$N$73:$P$75) + SUMPRODUCT(F64:H66,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="S43" s="6">
-        <f>SUMPRODUCT(G53:I55,$N$79:$P$81) + SUMPRODUCT(G42:I44,$N$73:$P$75) + SUMPRODUCT(G64:I66,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="T43" s="6">
-        <f>SUMPRODUCT(H53:J55,$N$79:$P$81) + SUMPRODUCT(H42:J44,$N$73:$P$75) + SUMPRODUCT(H64:J66,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="U43" s="6">
-        <f>SUMPRODUCT(I53:K55,$N$79:$P$81) + SUMPRODUCT(I42:K44,$N$73:$P$75) + SUMPRODUCT(I64:K66,$N$85:$P$87) + $S$73</f>
+        <f t="shared" si="16"/>
         <v>325.00110000000001</v>
       </c>
       <c r="V43" s="6"/>
@@ -5954,11 +5954,11 @@
       <c r="AI43" s="6"/>
       <c r="AJ43" s="7"/>
       <c r="AL43" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>55</v>
       </c>
       <c r="AM43" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>324.99999999999994</v>
       </c>
     </row>
@@ -6066,11 +6066,11 @@
       <c r="AI45" s="6"/>
       <c r="AJ45" s="7"/>
       <c r="AL45" s="1">
-        <f t="shared" ref="AL45:AL49" si="14">AD16</f>
+        <f t="shared" ref="AL45:AL49" si="20">AD16</f>
         <v>55</v>
       </c>
       <c r="AM45" s="1">
-        <f t="shared" ref="AM45:AM49" si="15">AD49</f>
+        <f t="shared" ref="AM45:AM49" si="21">AD49</f>
         <v>324.99999999999994</v>
       </c>
     </row>
@@ -6132,11 +6132,11 @@
       <c r="AI46" s="6"/>
       <c r="AJ46" s="7"/>
       <c r="AL46" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>55</v>
       </c>
       <c r="AM46" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>324.99999999999994</v>
       </c>
       <c r="AO46" s="1" t="s">
@@ -6178,35 +6178,35 @@
       <c r="L47" s="6"/>
       <c r="M47" s="6"/>
       <c r="N47" s="6">
-        <f>SUMPRODUCT(B46:D48,$U$79:$W$81) + SUMPRODUCT(B35:D37,$U$73:$W$75) + SUMPRODUCT(B57:D59,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" ref="N47:U54" si="22">SUMPRODUCT(B46:D48,$U$79:$W$81) + SUMPRODUCT(B35:D37,$U$73:$W$75) + SUMPRODUCT(B57:D59,$U$85:$W$87) + $Z$73</f>
         <v>325</v>
       </c>
       <c r="O47" s="6">
-        <f>SUMPRODUCT(C46:E48,$U$79:$W$81) + SUMPRODUCT(C35:E37,$U$73:$W$75) + SUMPRODUCT(C57:E59,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="P47" s="6">
-        <f>SUMPRODUCT(D46:F48,$U$79:$W$81) + SUMPRODUCT(D35:F37,$U$73:$W$75) + SUMPRODUCT(D57:F59,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="Q47" s="6">
-        <f>SUMPRODUCT(E46:G48,$U$79:$W$81) + SUMPRODUCT(E35:G37,$U$73:$W$75) + SUMPRODUCT(E57:G59,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="R47" s="6">
-        <f>SUMPRODUCT(F46:H48,$U$79:$W$81) + SUMPRODUCT(F35:H37,$U$73:$W$75) + SUMPRODUCT(F57:H59,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="S47" s="6">
-        <f>SUMPRODUCT(G46:I48,$U$79:$W$81) + SUMPRODUCT(G35:I37,$U$73:$W$75) + SUMPRODUCT(G57:I59,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="T47" s="6">
-        <f>SUMPRODUCT(H46:J48,$U$79:$W$81) + SUMPRODUCT(H35:J37,$U$73:$W$75) + SUMPRODUCT(H57:J59,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="U47" s="6">
-        <f>SUMPRODUCT(I46:K48,$U$79:$W$81) + SUMPRODUCT(I35:K37,$U$73:$W$75) + SUMPRODUCT(I57:K59,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="V47" s="6"/>
@@ -6225,11 +6225,11 @@
       <c r="AI47" s="6"/>
       <c r="AJ47" s="7"/>
       <c r="AL47" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>55</v>
       </c>
       <c r="AM47" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>324.99999999999994</v>
       </c>
     </row>
@@ -6268,35 +6268,35 @@
       <c r="L48" s="6"/>
       <c r="M48" s="6"/>
       <c r="N48" s="6">
-        <f>SUMPRODUCT(B47:D49,$U$79:$W$81) + SUMPRODUCT(B36:D38,$U$73:$W$75) + SUMPRODUCT(B58:D60,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="O48" s="6">
-        <f>SUMPRODUCT(C47:E49,$U$79:$W$81) + SUMPRODUCT(C36:E38,$U$73:$W$75) + SUMPRODUCT(C58:E60,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="P48" s="6">
-        <f>SUMPRODUCT(D47:F49,$U$79:$W$81) + SUMPRODUCT(D36:F38,$U$73:$W$75) + SUMPRODUCT(D58:F60,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="Q48" s="6">
-        <f>SUMPRODUCT(E47:G49,$U$79:$W$81) + SUMPRODUCT(E36:G38,$U$73:$W$75) + SUMPRODUCT(E58:G60,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="R48" s="6">
-        <f>SUMPRODUCT(F47:H49,$U$79:$W$81) + SUMPRODUCT(F36:H38,$U$73:$W$75) + SUMPRODUCT(F58:H60,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="S48" s="6">
-        <f>SUMPRODUCT(G47:I49,$U$79:$W$81) + SUMPRODUCT(G36:I38,$U$73:$W$75) + SUMPRODUCT(G58:I60,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="T48" s="6">
-        <f>SUMPRODUCT(H47:J49,$U$79:$W$81) + SUMPRODUCT(H36:J38,$U$73:$W$75) + SUMPRODUCT(H58:J60,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="U48" s="6">
-        <f>SUMPRODUCT(I47:K49,$U$79:$W$81) + SUMPRODUCT(I36:K38,$U$73:$W$75) + SUMPRODUCT(I58:K60,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="V48" s="6"/>
@@ -6307,37 +6307,37 @@
       <c r="AA48" s="7"/>
       <c r="AB48" s="5"/>
       <c r="AC48" s="6">
-        <f>SUMPRODUCT(N47:P49,$AC$73:$AE$75)</f>
+        <f t="shared" ref="AC48:AH53" si="23">SUMPRODUCT(N47:P49,$AC$73:$AE$75)</f>
         <v>324.99999999999994</v>
       </c>
       <c r="AD48" s="6">
-        <f>SUMPRODUCT(O47:Q49,$AC$73:$AE$75)</f>
+        <f t="shared" si="23"/>
         <v>324.99999999999994</v>
       </c>
       <c r="AE48" s="6">
-        <f>SUMPRODUCT(P47:R49,$AC$73:$AE$75)</f>
+        <f t="shared" si="23"/>
         <v>324.99999999999994</v>
       </c>
       <c r="AF48" s="6">
-        <f>SUMPRODUCT(Q47:S49,$AC$73:$AE$75)</f>
+        <f t="shared" si="23"/>
         <v>324.99999999999994</v>
       </c>
       <c r="AG48" s="6">
-        <f>SUMPRODUCT(R47:T49,$AC$73:$AE$75)</f>
+        <f t="shared" si="23"/>
         <v>324.99999999999994</v>
       </c>
       <c r="AH48" s="6">
-        <f>SUMPRODUCT(S47:U49,$AC$73:$AE$75)</f>
+        <f t="shared" si="23"/>
         <v>324.99999999999994</v>
       </c>
       <c r="AI48" s="6"/>
       <c r="AJ48" s="7"/>
       <c r="AL48" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>55</v>
       </c>
       <c r="AM48" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>324.99999999999994</v>
       </c>
       <c r="AO48" s="1">
@@ -6592,35 +6592,35 @@
       <c r="L49" s="6"/>
       <c r="M49" s="6"/>
       <c r="N49" s="6">
-        <f>SUMPRODUCT(B48:D50,$U$79:$W$81) + SUMPRODUCT(B37:D39,$U$73:$W$75) + SUMPRODUCT(B59:D61,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="O49" s="6">
-        <f>SUMPRODUCT(C48:E50,$U$79:$W$81) + SUMPRODUCT(C37:E39,$U$73:$W$75) + SUMPRODUCT(C59:E61,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="P49" s="6">
-        <f>SUMPRODUCT(D48:F50,$U$79:$W$81) + SUMPRODUCT(D37:F39,$U$73:$W$75) + SUMPRODUCT(D59:F61,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="Q49" s="6">
-        <f>SUMPRODUCT(E48:G50,$U$79:$W$81) + SUMPRODUCT(E37:G39,$U$73:$W$75) + SUMPRODUCT(E59:G61,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="R49" s="6">
-        <f>SUMPRODUCT(F48:H50,$U$79:$W$81) + SUMPRODUCT(F37:H39,$U$73:$W$75) + SUMPRODUCT(F59:H61,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="S49" s="6">
-        <f>SUMPRODUCT(G48:I50,$U$79:$W$81) + SUMPRODUCT(G37:I39,$U$73:$W$75) + SUMPRODUCT(G59:I61,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="T49" s="6">
-        <f>SUMPRODUCT(H48:J50,$U$79:$W$81) + SUMPRODUCT(H37:J39,$U$73:$W$75) + SUMPRODUCT(H59:J61,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="U49" s="6">
-        <f>SUMPRODUCT(I48:K50,$U$79:$W$81) + SUMPRODUCT(I37:K39,$U$73:$W$75) + SUMPRODUCT(I59:K61,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="V49" s="6"/>
@@ -6631,37 +6631,37 @@
       <c r="AA49" s="7"/>
       <c r="AB49" s="5"/>
       <c r="AC49" s="6">
-        <f>SUMPRODUCT(N48:P50,$AC$73:$AE$75)</f>
+        <f t="shared" si="23"/>
         <v>324.99999999999994</v>
       </c>
       <c r="AD49" s="6">
-        <f>SUMPRODUCT(O48:Q50,$AC$73:$AE$75)</f>
+        <f t="shared" si="23"/>
         <v>324.99999999999994</v>
       </c>
       <c r="AE49" s="6">
-        <f>SUMPRODUCT(P48:R50,$AC$73:$AE$75)</f>
+        <f t="shared" si="23"/>
         <v>324.99999999999994</v>
       </c>
       <c r="AF49" s="6">
-        <f>SUMPRODUCT(Q48:S50,$AC$73:$AE$75)</f>
+        <f t="shared" si="23"/>
         <v>324.99999999999994</v>
       </c>
       <c r="AG49" s="6">
-        <f>SUMPRODUCT(R48:T50,$AC$73:$AE$75)</f>
+        <f t="shared" si="23"/>
         <v>324.99999999999994</v>
       </c>
       <c r="AH49" s="6">
-        <f>SUMPRODUCT(S48:U50,$AC$73:$AE$75)</f>
+        <f t="shared" si="23"/>
         <v>324.99999999999994</v>
       </c>
       <c r="AI49" s="6"/>
       <c r="AJ49" s="7"/>
       <c r="AL49" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>55</v>
       </c>
       <c r="AM49" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>324.99999999999994</v>
       </c>
       <c r="AO49" s="1">
@@ -6916,35 +6916,35 @@
       <c r="L50" s="6"/>
       <c r="M50" s="6"/>
       <c r="N50" s="6">
-        <f>SUMPRODUCT(B49:D51,$U$79:$W$81) + SUMPRODUCT(B38:D40,$U$73:$W$75) + SUMPRODUCT(B60:D62,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="O50" s="6">
-        <f>SUMPRODUCT(C49:E51,$U$79:$W$81) + SUMPRODUCT(C38:E40,$U$73:$W$75) + SUMPRODUCT(C60:E62,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="P50" s="6">
-        <f>SUMPRODUCT(D49:F51,$U$79:$W$81) + SUMPRODUCT(D38:F40,$U$73:$W$75) + SUMPRODUCT(D60:F62,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="Q50" s="6">
-        <f>SUMPRODUCT(E49:G51,$U$79:$W$81) + SUMPRODUCT(E38:G40,$U$73:$W$75) + SUMPRODUCT(E60:G62,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="R50" s="6">
-        <f>SUMPRODUCT(F49:H51,$U$79:$W$81) + SUMPRODUCT(F38:H40,$U$73:$W$75) + SUMPRODUCT(F60:H62,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="S50" s="6">
-        <f>SUMPRODUCT(G49:I51,$U$79:$W$81) + SUMPRODUCT(G38:I40,$U$73:$W$75) + SUMPRODUCT(G60:I62,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="T50" s="6">
-        <f>SUMPRODUCT(H49:J51,$U$79:$W$81) + SUMPRODUCT(H38:J40,$U$73:$W$75) + SUMPRODUCT(H60:J62,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="U50" s="6">
-        <f>SUMPRODUCT(I49:K51,$U$79:$W$81) + SUMPRODUCT(I38:K40,$U$73:$W$75) + SUMPRODUCT(I60:K62,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="V50" s="6"/>
@@ -6955,27 +6955,27 @@
       <c r="AA50" s="7"/>
       <c r="AB50" s="5"/>
       <c r="AC50" s="6">
-        <f>SUMPRODUCT(N49:P51,$AC$73:$AE$75)</f>
+        <f t="shared" si="23"/>
         <v>324.99999999999994</v>
       </c>
       <c r="AD50" s="6">
-        <f>SUMPRODUCT(O49:Q51,$AC$73:$AE$75)</f>
+        <f t="shared" si="23"/>
         <v>324.99999999999994</v>
       </c>
       <c r="AE50" s="6">
-        <f>SUMPRODUCT(P49:R51,$AC$73:$AE$75)</f>
+        <f t="shared" si="23"/>
         <v>324.99999999999994</v>
       </c>
       <c r="AF50" s="6">
-        <f>SUMPRODUCT(Q49:S51,$AC$73:$AE$75)</f>
+        <f t="shared" si="23"/>
         <v>324.99999999999994</v>
       </c>
       <c r="AG50" s="6">
-        <f>SUMPRODUCT(R49:T51,$AC$73:$AE$75)</f>
+        <f t="shared" si="23"/>
         <v>324.99999999999994</v>
       </c>
       <c r="AH50" s="6">
-        <f>SUMPRODUCT(S49:U51,$AC$73:$AE$75)</f>
+        <f t="shared" si="23"/>
         <v>324.99999999999994</v>
       </c>
       <c r="AI50" s="6"/>
@@ -7024,35 +7024,35 @@
       <c r="L51" s="6"/>
       <c r="M51" s="6"/>
       <c r="N51" s="6">
-        <f>SUMPRODUCT(B50:D52,$U$79:$W$81) + SUMPRODUCT(B39:D41,$U$73:$W$75) + SUMPRODUCT(B61:D63,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="O51" s="6">
-        <f>SUMPRODUCT(C50:E52,$U$79:$W$81) + SUMPRODUCT(C39:E41,$U$73:$W$75) + SUMPRODUCT(C61:E63,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="P51" s="6">
-        <f>SUMPRODUCT(D50:F52,$U$79:$W$81) + SUMPRODUCT(D39:F41,$U$73:$W$75) + SUMPRODUCT(D61:F63,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="Q51" s="6">
-        <f>SUMPRODUCT(E50:G52,$U$79:$W$81) + SUMPRODUCT(E39:G41,$U$73:$W$75) + SUMPRODUCT(E61:G63,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="R51" s="6">
-        <f>SUMPRODUCT(F50:H52,$U$79:$W$81) + SUMPRODUCT(F39:H41,$U$73:$W$75) + SUMPRODUCT(F61:H63,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="S51" s="6">
-        <f>SUMPRODUCT(G50:I52,$U$79:$W$81) + SUMPRODUCT(G39:I41,$U$73:$W$75) + SUMPRODUCT(G61:I63,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="T51" s="6">
-        <f>SUMPRODUCT(H50:J52,$U$79:$W$81) + SUMPRODUCT(H39:J41,$U$73:$W$75) + SUMPRODUCT(H61:J63,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="U51" s="6">
-        <f>SUMPRODUCT(I50:K52,$U$79:$W$81) + SUMPRODUCT(I39:K41,$U$73:$W$75) + SUMPRODUCT(I61:K63,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="V51" s="6"/>
@@ -7063,37 +7063,37 @@
       <c r="AA51" s="7"/>
       <c r="AB51" s="5"/>
       <c r="AC51" s="6">
-        <f>SUMPRODUCT(N50:P52,$AC$73:$AE$75)</f>
+        <f t="shared" si="23"/>
         <v>324.99999999999994</v>
       </c>
       <c r="AD51" s="6">
-        <f>SUMPRODUCT(O50:Q52,$AC$73:$AE$75)</f>
+        <f t="shared" si="23"/>
         <v>324.99999999999994</v>
       </c>
       <c r="AE51" s="6">
-        <f>SUMPRODUCT(P50:R52,$AC$73:$AE$75)</f>
+        <f t="shared" si="23"/>
         <v>324.99999999999994</v>
       </c>
       <c r="AF51" s="6">
-        <f>SUMPRODUCT(Q50:S52,$AC$73:$AE$75)</f>
+        <f t="shared" si="23"/>
         <v>324.99999999999994</v>
       </c>
       <c r="AG51" s="6">
-        <f>SUMPRODUCT(R50:T52,$AC$73:$AE$75)</f>
+        <f t="shared" si="23"/>
         <v>324.99999999999994</v>
       </c>
       <c r="AH51" s="6">
-        <f>SUMPRODUCT(S50:U52,$AC$73:$AE$75)</f>
+        <f t="shared" si="23"/>
         <v>324.99999999999994</v>
       </c>
       <c r="AI51" s="6"/>
       <c r="AJ51" s="7"/>
       <c r="AL51" s="1">
-        <f t="shared" ref="AL51:AL55" si="16">AE16</f>
+        <f t="shared" ref="AL51:AL55" si="24">AE16</f>
         <v>55</v>
       </c>
       <c r="AM51" s="1">
-        <f t="shared" ref="AM51:AM55" si="17">AE49</f>
+        <f t="shared" ref="AM51:AM55" si="25">AE49</f>
         <v>324.99999999999994</v>
       </c>
       <c r="AO51" s="1" t="s">
@@ -7135,35 +7135,35 @@
       <c r="L52" s="6"/>
       <c r="M52" s="6"/>
       <c r="N52" s="6">
-        <f>SUMPRODUCT(B51:D53,$U$79:$W$81) + SUMPRODUCT(B40:D42,$U$73:$W$75) + SUMPRODUCT(B62:D64,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="O52" s="6">
-        <f>SUMPRODUCT(C51:E53,$U$79:$W$81) + SUMPRODUCT(C40:E42,$U$73:$W$75) + SUMPRODUCT(C62:E64,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="P52" s="6">
-        <f>SUMPRODUCT(D51:F53,$U$79:$W$81) + SUMPRODUCT(D40:F42,$U$73:$W$75) + SUMPRODUCT(D62:F64,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="Q52" s="6">
-        <f>SUMPRODUCT(E51:G53,$U$79:$W$81) + SUMPRODUCT(E40:G42,$U$73:$W$75) + SUMPRODUCT(E62:G64,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="R52" s="6">
-        <f>SUMPRODUCT(F51:H53,$U$79:$W$81) + SUMPRODUCT(F40:H42,$U$73:$W$75) + SUMPRODUCT(F62:H64,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="S52" s="6">
-        <f>SUMPRODUCT(G51:I53,$U$79:$W$81) + SUMPRODUCT(G40:I42,$U$73:$W$75) + SUMPRODUCT(G62:I64,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="T52" s="6">
-        <f>SUMPRODUCT(H51:J53,$U$79:$W$81) + SUMPRODUCT(H40:J42,$U$73:$W$75) + SUMPRODUCT(H62:J64,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="U52" s="6">
-        <f>SUMPRODUCT(I51:K53,$U$79:$W$81) + SUMPRODUCT(I40:K42,$U$73:$W$75) + SUMPRODUCT(I62:K64,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="V52" s="6"/>
@@ -7174,37 +7174,37 @@
       <c r="AA52" s="7"/>
       <c r="AB52" s="5"/>
       <c r="AC52" s="6">
-        <f>SUMPRODUCT(N51:P53,$AC$73:$AE$75)</f>
+        <f t="shared" si="23"/>
         <v>324.99999999999994</v>
       </c>
       <c r="AD52" s="6">
-        <f>SUMPRODUCT(O51:Q53,$AC$73:$AE$75)</f>
+        <f t="shared" si="23"/>
         <v>324.99999999999994</v>
       </c>
       <c r="AE52" s="6">
-        <f>SUMPRODUCT(P51:R53,$AC$73:$AE$75)</f>
+        <f t="shared" si="23"/>
         <v>324.99999999999994</v>
       </c>
       <c r="AF52" s="6">
-        <f>SUMPRODUCT(Q51:S53,$AC$73:$AE$75)</f>
+        <f t="shared" si="23"/>
         <v>324.99999999999994</v>
       </c>
       <c r="AG52" s="6">
-        <f>SUMPRODUCT(R51:T53,$AC$73:$AE$75)</f>
+        <f t="shared" si="23"/>
         <v>324.99999999999994</v>
       </c>
       <c r="AH52" s="6">
-        <f>SUMPRODUCT(S51:U53,$AC$73:$AE$75)</f>
+        <f t="shared" si="23"/>
         <v>324.99999999999994</v>
       </c>
       <c r="AI52" s="6"/>
       <c r="AJ52" s="7"/>
       <c r="AL52" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="24"/>
         <v>55</v>
       </c>
       <c r="AM52" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="25"/>
         <v>324.99999999999994</v>
       </c>
       <c r="AO52" s="1">
@@ -7246,35 +7246,35 @@
       <c r="L53" s="6"/>
       <c r="M53" s="6"/>
       <c r="N53" s="6">
-        <f>SUMPRODUCT(B52:D54,$U$79:$W$81) + SUMPRODUCT(B41:D43,$U$73:$W$75) + SUMPRODUCT(B63:D65,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="O53" s="6">
-        <f>SUMPRODUCT(C52:E54,$U$79:$W$81) + SUMPRODUCT(C41:E43,$U$73:$W$75) + SUMPRODUCT(C63:E65,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="P53" s="6">
-        <f>SUMPRODUCT(D52:F54,$U$79:$W$81) + SUMPRODUCT(D41:F43,$U$73:$W$75) + SUMPRODUCT(D63:F65,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="Q53" s="6">
-        <f>SUMPRODUCT(E52:G54,$U$79:$W$81) + SUMPRODUCT(E41:G43,$U$73:$W$75) + SUMPRODUCT(E63:G65,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="R53" s="6">
-        <f>SUMPRODUCT(F52:H54,$U$79:$W$81) + SUMPRODUCT(F41:H43,$U$73:$W$75) + SUMPRODUCT(F63:H65,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="S53" s="6">
-        <f>SUMPRODUCT(G52:I54,$U$79:$W$81) + SUMPRODUCT(G41:I43,$U$73:$W$75) + SUMPRODUCT(G63:I65,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="T53" s="6">
-        <f>SUMPRODUCT(H52:J54,$U$79:$W$81) + SUMPRODUCT(H41:J43,$U$73:$W$75) + SUMPRODUCT(H63:J65,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="U53" s="6">
-        <f>SUMPRODUCT(I52:K54,$U$79:$W$81) + SUMPRODUCT(I41:K43,$U$73:$W$75) + SUMPRODUCT(I63:K65,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="V53" s="6"/>
@@ -7285,37 +7285,37 @@
       <c r="AA53" s="7"/>
       <c r="AB53" s="5"/>
       <c r="AC53" s="6">
-        <f>SUMPRODUCT(N52:P54,$AC$73:$AE$75)</f>
+        <f t="shared" si="23"/>
         <v>324.99999999999994</v>
       </c>
       <c r="AD53" s="6">
-        <f>SUMPRODUCT(O52:Q54,$AC$73:$AE$75)</f>
+        <f t="shared" si="23"/>
         <v>324.99999999999994</v>
       </c>
       <c r="AE53" s="6">
-        <f>SUMPRODUCT(P52:R54,$AC$73:$AE$75)</f>
+        <f t="shared" si="23"/>
         <v>324.99999999999994</v>
       </c>
       <c r="AF53" s="6">
-        <f>SUMPRODUCT(Q52:S54,$AC$73:$AE$75)</f>
+        <f t="shared" si="23"/>
         <v>324.99999999999994</v>
       </c>
       <c r="AG53" s="6">
-        <f>SUMPRODUCT(R52:T54,$AC$73:$AE$75)</f>
+        <f t="shared" si="23"/>
         <v>324.99999999999994</v>
       </c>
       <c r="AH53" s="6">
-        <f>SUMPRODUCT(S52:U54,$AC$73:$AE$75)</f>
+        <f t="shared" si="23"/>
         <v>324.99999999999994</v>
       </c>
       <c r="AI53" s="6"/>
       <c r="AJ53" s="7"/>
       <c r="AL53" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="24"/>
         <v>55</v>
       </c>
       <c r="AM53" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="25"/>
         <v>324.99999999999994</v>
       </c>
       <c r="AO53" s="1">
@@ -7357,35 +7357,35 @@
       <c r="L54" s="6"/>
       <c r="M54" s="6"/>
       <c r="N54" s="6">
-        <f>SUMPRODUCT(B53:D55,$U$79:$W$81) + SUMPRODUCT(B42:D44,$U$73:$W$75) + SUMPRODUCT(B64:D66,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="O54" s="6">
-        <f>SUMPRODUCT(C53:E55,$U$79:$W$81) + SUMPRODUCT(C42:E44,$U$73:$W$75) + SUMPRODUCT(C64:E66,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="P54" s="6">
-        <f>SUMPRODUCT(D53:F55,$U$79:$W$81) + SUMPRODUCT(D42:F44,$U$73:$W$75) + SUMPRODUCT(D64:F66,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="Q54" s="6">
-        <f>SUMPRODUCT(E53:G55,$U$79:$W$81) + SUMPRODUCT(E42:G44,$U$73:$W$75) + SUMPRODUCT(E64:G66,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="R54" s="6">
-        <f>SUMPRODUCT(F53:H55,$U$79:$W$81) + SUMPRODUCT(F42:H44,$U$73:$W$75) + SUMPRODUCT(F64:H66,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="S54" s="6">
-        <f>SUMPRODUCT(G53:I55,$U$79:$W$81) + SUMPRODUCT(G42:I44,$U$73:$W$75) + SUMPRODUCT(G64:I66,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="T54" s="6">
-        <f>SUMPRODUCT(H53:J55,$U$79:$W$81) + SUMPRODUCT(H42:J44,$U$73:$W$75) + SUMPRODUCT(H64:J66,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="U54" s="6">
-        <f>SUMPRODUCT(I53:K55,$U$79:$W$81) + SUMPRODUCT(I42:K44,$U$73:$W$75) + SUMPRODUCT(I64:K66,$U$85:$W$87) + $Z$73</f>
+        <f t="shared" si="22"/>
         <v>325</v>
       </c>
       <c r="V54" s="6"/>
@@ -7404,11 +7404,11 @@
       <c r="AI54" s="6"/>
       <c r="AJ54" s="7"/>
       <c r="AL54" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="24"/>
         <v>55</v>
       </c>
       <c r="AM54" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="25"/>
         <v>324.99999999999994</v>
       </c>
     </row>
@@ -7470,11 +7470,11 @@
       <c r="AI55" s="6"/>
       <c r="AJ55" s="7"/>
       <c r="AL55" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="24"/>
         <v>55</v>
       </c>
       <c r="AM55" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="25"/>
         <v>324.99999999999994</v>
       </c>
     </row>
@@ -7585,11 +7585,11 @@
       <c r="AI57" s="6"/>
       <c r="AJ57" s="7"/>
       <c r="AL57" s="1">
-        <f t="shared" ref="AL57:AL61" si="18">AF16</f>
+        <f t="shared" ref="AL57:AL61" si="26">AF16</f>
         <v>55</v>
       </c>
       <c r="AM57" s="1">
-        <f t="shared" ref="AM57:AM61" si="19">AF49</f>
+        <f t="shared" ref="AM57:AM61" si="27">AF49</f>
         <v>324.99999999999994</v>
       </c>
       <c r="AO57" s="1">
@@ -7654,11 +7654,11 @@
       <c r="AI58" s="6"/>
       <c r="AJ58" s="7"/>
       <c r="AL58" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="26"/>
         <v>55</v>
       </c>
       <c r="AM58" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="27"/>
         <v>324.99999999999994</v>
       </c>
       <c r="AO58" s="1">
@@ -7723,11 +7723,11 @@
       <c r="AI59" s="6"/>
       <c r="AJ59" s="7"/>
       <c r="AL59" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="26"/>
         <v>55</v>
       </c>
       <c r="AM59" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="27"/>
         <v>324.99999999999994</v>
       </c>
     </row>
@@ -7789,11 +7789,11 @@
       <c r="AI60" s="6"/>
       <c r="AJ60" s="7"/>
       <c r="AL60" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="26"/>
         <v>55</v>
       </c>
       <c r="AM60" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="27"/>
         <v>324.99999999999994</v>
       </c>
       <c r="AO60" s="1" t="s">
@@ -7858,11 +7858,11 @@
       <c r="AI61" s="6"/>
       <c r="AJ61" s="7"/>
       <c r="AL61" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="26"/>
         <v>55</v>
       </c>
       <c r="AM61" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="27"/>
         <v>324.99999999999994</v>
       </c>
       <c r="AO61" s="1">
@@ -7996,11 +7996,11 @@
       <c r="AI63" s="6"/>
       <c r="AJ63" s="7"/>
       <c r="AL63" s="1">
-        <f t="shared" ref="AL63:AL67" si="20">AG16</f>
+        <f t="shared" ref="AL63:AL67" si="28">AG16</f>
         <v>55</v>
       </c>
       <c r="AM63" s="1">
-        <f t="shared" ref="AM63:AM67" si="21">AG49</f>
+        <f t="shared" ref="AM63:AM67" si="29">AG49</f>
         <v>324.99999999999994</v>
       </c>
     </row>
@@ -8062,11 +8062,11 @@
       <c r="AI64" s="6"/>
       <c r="AJ64" s="7"/>
       <c r="AL64" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="28"/>
         <v>55</v>
       </c>
       <c r="AM64" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="29"/>
         <v>324.99999999999994</v>
       </c>
     </row>
@@ -8128,11 +8128,11 @@
       <c r="AI65" s="6"/>
       <c r="AJ65" s="7"/>
       <c r="AL65" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="28"/>
         <v>55</v>
       </c>
       <c r="AM65" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="29"/>
         <v>324.99999999999994</v>
       </c>
     </row>
@@ -8194,11 +8194,11 @@
       <c r="AI66" s="6"/>
       <c r="AJ66" s="7"/>
       <c r="AL66" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="28"/>
         <v>55</v>
       </c>
       <c r="AM66" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="29"/>
         <v>324.99999999999994</v>
       </c>
     </row>
@@ -8240,11 +8240,11 @@
       <c r="AI67" s="6"/>
       <c r="AJ67" s="7"/>
       <c r="AL67" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="28"/>
         <v>55</v>
       </c>
       <c r="AM67" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="29"/>
         <v>324.99999999999994</v>
       </c>
     </row>
@@ -8332,11 +8332,11 @@
       <c r="AI69" s="6"/>
       <c r="AJ69" s="7"/>
       <c r="AL69" s="1">
-        <f t="shared" ref="AL69:AL73" si="22">AH16</f>
+        <f t="shared" ref="AL69:AL73" si="30">AH16</f>
         <v>55</v>
       </c>
       <c r="AM69" s="1">
-        <f t="shared" ref="AM69:AM73" si="23">AH49</f>
+        <f t="shared" ref="AM69:AM73" si="31">AH49</f>
         <v>324.99999999999994</v>
       </c>
     </row>
@@ -8378,11 +8378,11 @@
       <c r="AI70" s="6"/>
       <c r="AJ70" s="7"/>
       <c r="AL70" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>55</v>
       </c>
       <c r="AM70" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="31"/>
         <v>324.99999999999994</v>
       </c>
     </row>
@@ -8434,11 +8434,11 @@
       <c r="AI71" s="6"/>
       <c r="AJ71" s="7"/>
       <c r="AL71" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>55</v>
       </c>
       <c r="AM71" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="31"/>
         <v>324.99999999999994</v>
       </c>
     </row>
@@ -8480,11 +8480,11 @@
       <c r="AI72" s="6"/>
       <c r="AJ72" s="7"/>
       <c r="AL72" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>55</v>
       </c>
       <c r="AM72" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="31"/>
         <v>324.99999999999994</v>
       </c>
     </row>
@@ -8534,15 +8534,15 @@
       <c r="AA73" s="7"/>
       <c r="AB73" s="5"/>
       <c r="AC73" s="6">
-        <f t="shared" ref="AC73:AE75" si="24">1/9</f>
+        <f t="shared" ref="AC73:AE75" si="32">1/9</f>
         <v>0.1111111111111111</v>
       </c>
       <c r="AD73" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="32"/>
         <v>0.1111111111111111</v>
       </c>
       <c r="AE73" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="32"/>
         <v>0.1111111111111111</v>
       </c>
       <c r="AF73" s="6"/>
@@ -8551,11 +8551,11 @@
       <c r="AI73" s="6"/>
       <c r="AJ73" s="7"/>
       <c r="AL73" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>55</v>
       </c>
       <c r="AM73" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="31"/>
         <v>324.99999999999994</v>
       </c>
     </row>
@@ -8601,15 +8601,15 @@
       <c r="AA74" s="7"/>
       <c r="AB74" s="5"/>
       <c r="AC74" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="32"/>
         <v>0.1111111111111111</v>
       </c>
       <c r="AD74" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="32"/>
         <v>0.1111111111111111</v>
       </c>
       <c r="AE74" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="32"/>
         <v>0.1111111111111111</v>
       </c>
       <c r="AF74" s="6"/>
@@ -8660,15 +8660,15 @@
       <c r="AA75" s="7"/>
       <c r="AB75" s="5"/>
       <c r="AC75" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="32"/>
         <v>0.1111111111111111</v>
       </c>
       <c r="AD75" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="32"/>
         <v>0.1111111111111111</v>
       </c>
       <c r="AE75" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="32"/>
         <v>0.1111111111111111</v>
       </c>
       <c r="AF75" s="6"/>

</xml_diff>

<commit_message>
Tu Ko with two convolution layers and random input
</commit_message>
<xml_diff>
--- a/Book2.xlsx
+++ b/Book2.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\NeuralNetwork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{251E0D85-DAF1-4E3B-8171-3EF8245CCAE4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{745BD150-3A44-473D-AF6C-0F4B0F575BC8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Convolution One channel" sheetId="1" r:id="rId1"/>
     <sheet name="Convolution three channels" sheetId="3" r:id="rId2"/>
+    <sheet name="2 convolution layers" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179017" iterateDelta="1E-4"/>
   <extLst>
@@ -2181,7 +2182,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D771BA6-BDBF-4EDD-8045-037C0BFCFB28}">
   <dimension ref="A1:DH103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="Y1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AO4" sqref="AO4"/>
     </sheetView>
   </sheetViews>
@@ -9709,4 +9710,2364 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07A9D8FE-6989-4D43-B448-9A142F06CD0A}">
+  <dimension ref="B2:AC70"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="AC55" sqref="AC55"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <f>B2+7</f>
+        <v>7</v>
+      </c>
+      <c r="C3" s="1">
+        <f t="shared" ref="C3:H8" si="0">C2+7</f>
+        <v>8</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="E3" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F3" s="1">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="G3" s="1">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H3" s="1">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="K3">
+        <f>SUMPRODUCT(B2:D4,$C$13:$E$15)+$G$13</f>
+        <v>43</v>
+      </c>
+      <c r="L3" s="1">
+        <f t="shared" ref="L3:O3" si="1">SUMPRODUCT(C2:E4,$C$13:$E$15)+$G$13</f>
+        <v>46.6</v>
+      </c>
+      <c r="M3" s="1">
+        <f t="shared" si="1"/>
+        <v>50.199999999999996</v>
+      </c>
+      <c r="N3" s="1">
+        <f t="shared" si="1"/>
+        <v>53.8</v>
+      </c>
+      <c r="O3" s="1">
+        <f t="shared" si="1"/>
+        <v>57.4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
+        <f>B3+7</f>
+        <v>14</v>
+      </c>
+      <c r="C4" s="1">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="G4" s="1">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="K4" s="1">
+        <f t="shared" ref="K4:K7" si="2">SUMPRODUCT(B3:D5,$C$13:$E$15)+$G$13</f>
+        <v>68.199999999999989</v>
+      </c>
+      <c r="L4" s="1">
+        <f t="shared" ref="L4:L7" si="3">SUMPRODUCT(C3:E5,$C$13:$E$15)+$G$13</f>
+        <v>71.8</v>
+      </c>
+      <c r="M4" s="1">
+        <f t="shared" ref="M4:M7" si="4">SUMPRODUCT(D3:F5,$C$13:$E$15)+$G$13</f>
+        <v>75.400000000000006</v>
+      </c>
+      <c r="N4" s="1">
+        <f t="shared" ref="N4:N7" si="5">SUMPRODUCT(E3:G5,$C$13:$E$15)+$G$13</f>
+        <v>79</v>
+      </c>
+      <c r="O4" s="1">
+        <f t="shared" ref="O4:O7" si="6">SUMPRODUCT(F3:H5,$C$13:$E$15)+$G$13</f>
+        <v>82.6</v>
+      </c>
+      <c r="S4">
+        <f>SUMPRODUCT(K3:M5,$L$13:$N$15)+$P$13</f>
+        <v>307</v>
+      </c>
+      <c r="T4" s="1">
+        <f t="shared" ref="T4:U4" si="7">SUMPRODUCT(L3:N5,$L$13:$N$15)+$P$13</f>
+        <v>319.95999999999998</v>
+      </c>
+      <c r="U4" s="1">
+        <f t="shared" si="7"/>
+        <v>332.92</v>
+      </c>
+      <c r="X4">
+        <f>S4</f>
+        <v>307</v>
+      </c>
+      <c r="AA4">
+        <f t="array" ref="AA4:AA5">MMULT(TRANSPOSE(X15:Y23),X4:X12)</f>
+        <v>3696.12</v>
+      </c>
+      <c r="AB4">
+        <f>AA4+1</f>
+        <v>3697.12</v>
+      </c>
+      <c r="AC4">
+        <v>3700</v>
+      </c>
+    </row>
+    <row r="5" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <f>B4+7</f>
+        <v>21</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="K5" s="1">
+        <f t="shared" si="2"/>
+        <v>93.4</v>
+      </c>
+      <c r="L5" s="1">
+        <f t="shared" si="3"/>
+        <v>96.999999999999986</v>
+      </c>
+      <c r="M5" s="1">
+        <f t="shared" si="4"/>
+        <v>100.6</v>
+      </c>
+      <c r="N5" s="1">
+        <f t="shared" si="5"/>
+        <v>104.19999999999999</v>
+      </c>
+      <c r="O5" s="1">
+        <f t="shared" si="6"/>
+        <v>107.8</v>
+      </c>
+      <c r="S5" s="1">
+        <f t="shared" ref="S5:S6" si="8">SUMPRODUCT(K4:M6,$L$13:$N$15)+$P$13</f>
+        <v>397.71999999999997</v>
+      </c>
+      <c r="T5" s="1">
+        <f t="shared" ref="T5:T6" si="9">SUMPRODUCT(L4:N6,$L$13:$N$15)+$P$13</f>
+        <v>410.67999999999995</v>
+      </c>
+      <c r="U5" s="1">
+        <f t="shared" ref="U5:U6" si="10">SUMPRODUCT(M4:O6,$L$13:$N$15)+$P$13</f>
+        <v>423.64</v>
+      </c>
+      <c r="X5" s="1">
+        <f t="shared" ref="X5:X6" si="11">S5</f>
+        <v>397.71999999999997</v>
+      </c>
+      <c r="AA5">
+        <v>3696.12</v>
+      </c>
+      <c r="AB5" s="1">
+        <f>AA5+1</f>
+        <v>3697.12</v>
+      </c>
+      <c r="AC5">
+        <v>3690</v>
+      </c>
+    </row>
+    <row r="6" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <f>B5+7</f>
+        <v>28</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="K6" s="1">
+        <f t="shared" si="2"/>
+        <v>118.6</v>
+      </c>
+      <c r="L6" s="1">
+        <f t="shared" si="3"/>
+        <v>122.19999999999999</v>
+      </c>
+      <c r="M6" s="1">
+        <f t="shared" si="4"/>
+        <v>125.79999999999998</v>
+      </c>
+      <c r="N6" s="1">
+        <f t="shared" si="5"/>
+        <v>129.39999999999998</v>
+      </c>
+      <c r="O6" s="1">
+        <f t="shared" si="6"/>
+        <v>133</v>
+      </c>
+      <c r="S6" s="1">
+        <f t="shared" si="8"/>
+        <v>488.43999999999994</v>
+      </c>
+      <c r="T6" s="1">
+        <f t="shared" si="9"/>
+        <v>501.4</v>
+      </c>
+      <c r="U6" s="1">
+        <f t="shared" si="10"/>
+        <v>514.3599999999999</v>
+      </c>
+      <c r="X6" s="1">
+        <f t="shared" si="11"/>
+        <v>488.43999999999994</v>
+      </c>
+    </row>
+    <row r="7" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <f>B6+7</f>
+        <v>35</v>
+      </c>
+      <c r="C7" s="1">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="K7" s="1">
+        <f t="shared" si="2"/>
+        <v>143.79999999999998</v>
+      </c>
+      <c r="L7" s="1">
+        <f t="shared" si="3"/>
+        <v>147.39999999999998</v>
+      </c>
+      <c r="M7" s="1">
+        <f t="shared" si="4"/>
+        <v>151</v>
+      </c>
+      <c r="N7" s="1">
+        <f t="shared" si="5"/>
+        <v>154.6</v>
+      </c>
+      <c r="O7" s="1">
+        <f t="shared" si="6"/>
+        <v>158.19999999999999</v>
+      </c>
+      <c r="X7">
+        <f>T4</f>
+        <v>319.95999999999998</v>
+      </c>
+      <c r="AC7">
+        <f>AB4-AC4</f>
+        <v>-2.8800000000001091</v>
+      </c>
+    </row>
+    <row r="8" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <f>B7+7</f>
+        <v>42</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="X8" s="1">
+        <f t="shared" ref="X8:X9" si="12">T5</f>
+        <v>410.67999999999995</v>
+      </c>
+      <c r="AC8" s="1">
+        <f>AB5-AC5</f>
+        <v>7.1199999999998909</v>
+      </c>
+    </row>
+    <row r="9" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="X9" s="1">
+        <f t="shared" si="12"/>
+        <v>501.4</v>
+      </c>
+    </row>
+    <row r="10" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="X10">
+        <f>U4</f>
+        <v>332.92</v>
+      </c>
+    </row>
+    <row r="11" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="X11" s="1">
+        <f t="shared" ref="X11:X12" si="13">U5</f>
+        <v>423.64</v>
+      </c>
+    </row>
+    <row r="12" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="X12" s="1">
+        <f t="shared" si="13"/>
+        <v>514.3599999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <f>C13+0.1</f>
+        <v>0.1</v>
+      </c>
+      <c r="E13" s="1">
+        <f>D13+0.1</f>
+        <v>0.2</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="L13" s="1">
+        <v>0</v>
+      </c>
+      <c r="M13" s="1">
+        <f>L13+0.1</f>
+        <v>0.1</v>
+      </c>
+      <c r="N13" s="1">
+        <f>M13+0.1</f>
+        <v>0.2</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <f>C13+0.3</f>
+        <v>0.3</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" ref="D14:E15" si="14">C14+0.1</f>
+        <v>0.4</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="14"/>
+        <v>0.5</v>
+      </c>
+      <c r="L14" s="1">
+        <f>L13+0.3</f>
+        <v>0.3</v>
+      </c>
+      <c r="M14" s="1">
+        <f t="shared" ref="M14:N14" si="15">L14+0.1</f>
+        <v>0.4</v>
+      </c>
+      <c r="N14" s="1">
+        <f t="shared" si="15"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="C15" s="1">
+        <f>C14+0.3</f>
+        <v>0.6</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="14"/>
+        <v>0.7</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="14"/>
+        <v>0.79999999999999993</v>
+      </c>
+      <c r="L15" s="1">
+        <f>L14+0.3</f>
+        <v>0.6</v>
+      </c>
+      <c r="M15" s="1">
+        <f t="shared" ref="M15:N15" si="16">L15+0.1</f>
+        <v>0.7</v>
+      </c>
+      <c r="N15" s="1">
+        <f t="shared" si="16"/>
+        <v>0.79999999999999993</v>
+      </c>
+      <c r="X15">
+        <v>1</v>
+      </c>
+      <c r="Y15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="X16" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="X17" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <f>SUMPRODUCT(B2:F6,$K$24:$O$28)</f>
+        <v>1694.3039999999128</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" ref="D18:E18" si="17">SUMPRODUCT(C2:G6,$K$24:$O$28)</f>
+        <v>1831.6799999999057</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="17"/>
+        <v>1969.0559999998986</v>
+      </c>
+      <c r="L18">
+        <f>SUMPRODUCT($R$24:$T$26,K3:M5)</f>
+        <v>2739.8879999998589</v>
+      </c>
+      <c r="M18" s="1">
+        <f t="shared" ref="M18:N18" si="18">SUMPRODUCT($R$24:$T$26,L3:N5)</f>
+        <v>2877.2639999998519</v>
+      </c>
+      <c r="N18" s="1">
+        <f t="shared" si="18"/>
+        <v>3014.6399999998448</v>
+      </c>
+      <c r="X18" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="C19" s="1">
+        <f t="shared" ref="C19:C20" si="19">SUMPRODUCT(B3:F7,$K$24:$O$28)</f>
+        <v>2655.9359999998633</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" ref="D19:D20" si="20">SUMPRODUCT(C3:G7,$K$24:$O$28)</f>
+        <v>2793.3119999998562</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" ref="E19:E20" si="21">SUMPRODUCT(D3:H7,$K$24:$O$28)</f>
+        <v>2930.6879999998491</v>
+      </c>
+      <c r="L19" s="1">
+        <f t="shared" ref="L19:N19" si="22">SUMPRODUCT($R$24:$T$26,K4:M6)</f>
+        <v>3701.5199999998094</v>
+      </c>
+      <c r="M19" s="1">
+        <f t="shared" si="22"/>
+        <v>3838.8959999998024</v>
+      </c>
+      <c r="N19" s="1">
+        <f t="shared" si="22"/>
+        <v>3976.2719999997953</v>
+      </c>
+      <c r="X19" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="C20" s="1">
+        <f t="shared" si="19"/>
+        <v>3617.5679999998138</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="20"/>
+        <v>3754.9439999998067</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="21"/>
+        <v>3892.3199999997996</v>
+      </c>
+      <c r="L20" s="1">
+        <f t="shared" ref="L20:N20" si="23">SUMPRODUCT($R$24:$T$26,K5:M7)</f>
+        <v>4663.1519999997599</v>
+      </c>
+      <c r="M20" s="1">
+        <f t="shared" si="23"/>
+        <v>4800.5279999997529</v>
+      </c>
+      <c r="N20" s="1">
+        <f t="shared" si="23"/>
+        <v>4937.9039999997458</v>
+      </c>
+      <c r="X20" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="X21" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="X22" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="X23" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y23" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <f>SUMPRODUCT($C$13:$E$15,I22:K24)</f>
+        <v>2.7135999999998597</v>
+      </c>
+      <c r="C24" s="1">
+        <f t="shared" ref="C24:H24" si="24">SUMPRODUCT($C$13:$E$15,J22:L24)</f>
+        <v>7.4623999999996151</v>
+      </c>
+      <c r="D24" s="1">
+        <f t="shared" si="24"/>
+        <v>13.610399999999299</v>
+      </c>
+      <c r="E24" s="1">
+        <f t="shared" si="24"/>
+        <v>14.458399999999255</v>
+      </c>
+      <c r="F24" s="1">
+        <f t="shared" si="24"/>
+        <v>11.235999999999422</v>
+      </c>
+      <c r="G24" s="1">
+        <f t="shared" si="24"/>
+        <v>5.0879999999997381</v>
+      </c>
+      <c r="H24" s="1">
+        <f t="shared" si="24"/>
+        <v>1.5263999999999214</v>
+      </c>
+      <c r="K24">
+        <f>SUMPRODUCT(P22:R24,$L$13:$N$15)</f>
+        <v>3.3919999999998249</v>
+      </c>
+      <c r="L24" s="1">
+        <f t="shared" ref="L24:O24" si="25">SUMPRODUCT(Q22:S24,$L$13:$N$15)</f>
+        <v>6.3599999999996726</v>
+      </c>
+      <c r="M24" s="1">
+        <f t="shared" si="25"/>
+        <v>8.9039999999995416</v>
+      </c>
+      <c r="N24" s="1">
+        <f t="shared" si="25"/>
+        <v>5.5119999999997162</v>
+      </c>
+      <c r="O24" s="1">
+        <f t="shared" si="25"/>
+        <v>2.543999999999869</v>
+      </c>
+      <c r="R24">
+        <f>W24</f>
+        <v>4.2399999999997817</v>
+      </c>
+      <c r="S24">
+        <f>W27</f>
+        <v>4.2399999999997817</v>
+      </c>
+      <c r="T24">
+        <f>W30</f>
+        <v>4.2399999999997817</v>
+      </c>
+      <c r="W24">
+        <f t="array" ref="W24:W32">MMULT(X15:Y23,AC7:AC8)</f>
+        <v>4.2399999999997817</v>
+      </c>
+    </row>
+    <row r="25" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B25" s="1">
+        <f t="shared" ref="B25:B30" si="26">SUMPRODUCT($C$13:$E$15,I23:K25)</f>
+        <v>6.1055999999996855</v>
+      </c>
+      <c r="C25" s="1">
+        <f t="shared" ref="C25:C30" si="27">SUMPRODUCT($C$13:$E$15,J23:L25)</f>
+        <v>16.535999999999149</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" ref="D25:D30" si="28">SUMPRODUCT($C$13:$E$15,K23:M25)</f>
+        <v>29.637599999998471</v>
+      </c>
+      <c r="E25" s="1">
+        <f t="shared" ref="E25:E30" si="29">SUMPRODUCT($C$13:$E$15,L23:N25)</f>
+        <v>30.909599999998409</v>
+      </c>
+      <c r="F25" s="1">
+        <f t="shared" ref="F25:F30" si="30">SUMPRODUCT($C$13:$E$15,M23:O25)</f>
+        <v>23.531999999998789</v>
+      </c>
+      <c r="G25" s="1">
+        <f t="shared" ref="G25:G30" si="31">SUMPRODUCT($C$13:$E$15,N23:P25)</f>
+        <v>10.430399999999462</v>
+      </c>
+      <c r="H25" s="1">
+        <f t="shared" ref="H25:H30" si="32">SUMPRODUCT($C$13:$E$15,O23:Q25)</f>
+        <v>3.0527999999998428</v>
+      </c>
+      <c r="K25" s="1">
+        <f t="shared" ref="K25:K28" si="33">SUMPRODUCT(P23:R25,$L$13:$N$15)</f>
+        <v>5.5119999999997162</v>
+      </c>
+      <c r="L25" s="1">
+        <f t="shared" ref="L25:L28" si="34">SUMPRODUCT(Q23:S25,$L$13:$N$15)</f>
+        <v>10.175999999999476</v>
+      </c>
+      <c r="M25" s="1">
+        <f t="shared" ref="M25:M28" si="35">SUMPRODUCT(R23:T25,$L$13:$N$15)</f>
+        <v>13.99199999999928</v>
+      </c>
+      <c r="N25" s="1">
+        <f t="shared" ref="N25:N28" si="36">SUMPRODUCT(S23:U25,$L$13:$N$15)</f>
+        <v>8.4799999999995634</v>
+      </c>
+      <c r="O25" s="1">
+        <f t="shared" ref="O25:O28" si="37">SUMPRODUCT(T23:V25,$L$13:$N$15)</f>
+        <v>3.8159999999998035</v>
+      </c>
+      <c r="R25" s="1">
+        <f>W25</f>
+        <v>4.2399999999997817</v>
+      </c>
+      <c r="S25" s="1">
+        <f>W28</f>
+        <v>4.2399999999997817</v>
+      </c>
+      <c r="T25" s="1">
+        <f>W31</f>
+        <v>4.2399999999997817</v>
+      </c>
+      <c r="W25">
+        <v>4.2399999999997817</v>
+      </c>
+    </row>
+    <row r="26" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B26" s="1">
+        <f t="shared" si="26"/>
+        <v>8.5223999999995605</v>
+      </c>
+      <c r="C26" s="1">
+        <f t="shared" si="27"/>
+        <v>22.51439999999884</v>
+      </c>
+      <c r="D26" s="1">
+        <f t="shared" si="28"/>
+        <v>39.17759999999798</v>
+      </c>
+      <c r="E26" s="1">
+        <f t="shared" si="29"/>
+        <v>39.559199999997965</v>
+      </c>
+      <c r="F26" s="1">
+        <f t="shared" si="30"/>
+        <v>29.001599999998504</v>
+      </c>
+      <c r="G26" s="1">
+        <f t="shared" si="31"/>
+        <v>12.338399999999366</v>
+      </c>
+      <c r="H26" s="1">
+        <f t="shared" si="32"/>
+        <v>3.4343999999998229</v>
+      </c>
+      <c r="K26" s="1">
+        <f t="shared" si="33"/>
+        <v>6.3599999999996726</v>
+      </c>
+      <c r="L26" s="1">
+        <f t="shared" si="34"/>
+        <v>11.447999999999411</v>
+      </c>
+      <c r="M26" s="1">
+        <f t="shared" si="35"/>
+        <v>15.263999999999214</v>
+      </c>
+      <c r="N26" s="1">
+        <f t="shared" si="36"/>
+        <v>8.9039999999995416</v>
+      </c>
+      <c r="O26" s="1">
+        <f t="shared" si="37"/>
+        <v>3.8159999999998035</v>
+      </c>
+      <c r="R26" s="1">
+        <f>W26</f>
+        <v>4.2399999999997817</v>
+      </c>
+      <c r="S26" s="1">
+        <f>W29</f>
+        <v>4.2399999999997817</v>
+      </c>
+      <c r="T26" s="1">
+        <f>W32</f>
+        <v>4.2399999999997817</v>
+      </c>
+      <c r="W26">
+        <v>4.2399999999997817</v>
+      </c>
+    </row>
+    <row r="27" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B27" s="1">
+        <f t="shared" si="26"/>
+        <v>6.6567999999996577</v>
+      </c>
+      <c r="C27" s="1">
+        <f t="shared" si="27"/>
+        <v>17.002399999999124</v>
+      </c>
+      <c r="D27" s="1">
+        <f t="shared" si="28"/>
+        <v>28.36559999999854</v>
+      </c>
+      <c r="E27" s="1">
+        <f t="shared" si="29"/>
+        <v>27.305599999998595</v>
+      </c>
+      <c r="F27" s="1">
+        <f t="shared" si="30"/>
+        <v>18.867999999999029</v>
+      </c>
+      <c r="G27" s="1">
+        <f t="shared" si="31"/>
+        <v>7.5047999999996149</v>
+      </c>
+      <c r="H27" s="1">
+        <f t="shared" si="32"/>
+        <v>1.9079999999999018</v>
+      </c>
+      <c r="K27" s="1">
+        <f t="shared" si="33"/>
+        <v>2.9679999999998472</v>
+      </c>
+      <c r="L27" s="1">
+        <f t="shared" si="34"/>
+        <v>5.0879999999997381</v>
+      </c>
+      <c r="M27" s="1">
+        <f t="shared" si="35"/>
+        <v>6.3599999999996726</v>
+      </c>
+      <c r="N27" s="1">
+        <f t="shared" si="36"/>
+        <v>3.3919999999998254</v>
+      </c>
+      <c r="O27" s="1">
+        <f t="shared" si="37"/>
+        <v>1.2719999999999345</v>
+      </c>
+      <c r="W27">
+        <v>4.2399999999997817</v>
+      </c>
+    </row>
+    <row r="28" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B28" s="1">
+        <f t="shared" si="26"/>
+        <v>3.4343999999998234</v>
+      </c>
+      <c r="C28" s="1">
+        <f t="shared" si="27"/>
+        <v>8.2679999999995744</v>
+      </c>
+      <c r="D28" s="1">
+        <f t="shared" si="28"/>
+        <v>12.719999999999345</v>
+      </c>
+      <c r="E28" s="1">
+        <f t="shared" si="29"/>
+        <v>11.06639999999943</v>
+      </c>
+      <c r="F28" s="1">
+        <f t="shared" si="30"/>
+        <v>6.6143999999996597</v>
+      </c>
+      <c r="G28" s="1">
+        <f t="shared" si="31"/>
+        <v>2.1623999999998889</v>
+      </c>
+      <c r="H28" s="1">
+        <f t="shared" si="32"/>
+        <v>0.38159999999998034</v>
+      </c>
+      <c r="K28" s="1">
+        <f t="shared" si="33"/>
+        <v>0.84799999999995634</v>
+      </c>
+      <c r="L28" s="1">
+        <f t="shared" si="34"/>
+        <v>1.2719999999999345</v>
+      </c>
+      <c r="M28" s="1">
+        <f t="shared" si="35"/>
+        <v>1.2719999999999345</v>
+      </c>
+      <c r="N28" s="1">
+        <f t="shared" si="36"/>
+        <v>0.42399999999997817</v>
+      </c>
+      <c r="O28" s="1">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="W28">
+        <v>4.2399999999997817</v>
+      </c>
+    </row>
+    <row r="29" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B29" s="1">
+        <f t="shared" si="26"/>
+        <v>1.0175999999999477</v>
+      </c>
+      <c r="C29" s="1">
+        <f t="shared" si="27"/>
+        <v>2.2895999999998824</v>
+      </c>
+      <c r="D29" s="1">
+        <f t="shared" si="28"/>
+        <v>3.1799999999998363</v>
+      </c>
+      <c r="E29" s="1">
+        <f t="shared" si="29"/>
+        <v>2.4167999999998759</v>
+      </c>
+      <c r="F29" s="1">
+        <f t="shared" si="30"/>
+        <v>1.1447999999999412</v>
+      </c>
+      <c r="G29" s="1">
+        <f t="shared" si="31"/>
+        <v>0.25439999999998691</v>
+      </c>
+      <c r="H29" s="1">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="W29">
+        <v>4.2399999999997817</v>
+      </c>
+    </row>
+    <row r="30" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B30" s="1">
+        <f t="shared" si="26"/>
+        <v>0.16959999999999129</v>
+      </c>
+      <c r="C30" s="1">
+        <f t="shared" si="27"/>
+        <v>0.33919999999998257</v>
+      </c>
+      <c r="D30" s="1">
+        <f t="shared" si="28"/>
+        <v>0.3815999999999804</v>
+      </c>
+      <c r="E30" s="1">
+        <f t="shared" si="29"/>
+        <v>0.21199999999998909</v>
+      </c>
+      <c r="F30" s="1">
+        <f t="shared" si="30"/>
+        <v>4.2399999999997821E-2</v>
+      </c>
+      <c r="G30" s="1">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="H30" s="1">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="W30">
+        <v>4.2399999999997817</v>
+      </c>
+    </row>
+    <row r="31" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="W31">
+        <v>4.2399999999997817</v>
+      </c>
+    </row>
+    <row r="32" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="W32">
+        <v>4.2399999999997817</v>
+      </c>
+    </row>
+    <row r="33" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+    </row>
+    <row r="40" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B40" s="1">
+        <v>0</v>
+      </c>
+      <c r="C40" s="1">
+        <v>1</v>
+      </c>
+      <c r="D40" s="1">
+        <v>2</v>
+      </c>
+      <c r="E40" s="1">
+        <v>3</v>
+      </c>
+      <c r="F40" s="1">
+        <v>4</v>
+      </c>
+      <c r="G40" s="1">
+        <v>5</v>
+      </c>
+      <c r="H40" s="1">
+        <v>6</v>
+      </c>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
+      <c r="O40" s="1"/>
+      <c r="P40" s="1"/>
+      <c r="Q40" s="1"/>
+      <c r="R40" s="1"/>
+      <c r="S40" s="1"/>
+      <c r="T40" s="1"/>
+      <c r="U40" s="1"/>
+      <c r="V40" s="1"/>
+      <c r="W40" s="1"/>
+      <c r="X40" s="1"/>
+      <c r="Y40" s="1"/>
+      <c r="Z40" s="1"/>
+      <c r="AA40" s="1"/>
+      <c r="AB40" s="1"/>
+      <c r="AC40" s="1"/>
+    </row>
+    <row r="41" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B41" s="1">
+        <f>B40+7</f>
+        <v>7</v>
+      </c>
+      <c r="C41" s="1">
+        <f t="shared" ref="C41:C46" si="38">C40+7</f>
+        <v>8</v>
+      </c>
+      <c r="D41" s="1">
+        <f t="shared" ref="D41:D46" si="39">D40+7</f>
+        <v>9</v>
+      </c>
+      <c r="E41" s="1">
+        <f t="shared" ref="E41:E46" si="40">E40+7</f>
+        <v>10</v>
+      </c>
+      <c r="F41" s="1">
+        <f t="shared" ref="F41:F46" si="41">F40+7</f>
+        <v>11</v>
+      </c>
+      <c r="G41" s="1">
+        <f t="shared" ref="G41:G46" si="42">G40+7</f>
+        <v>12</v>
+      </c>
+      <c r="H41" s="1">
+        <f t="shared" ref="H41:H46" si="43">H40+7</f>
+        <v>13</v>
+      </c>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1">
+        <f>SUMPRODUCT(B40:D42,$C$51:$E$53)+$G$51</f>
+        <v>43</v>
+      </c>
+      <c r="L41" s="1">
+        <f t="shared" ref="L41:O41" si="44">SUMPRODUCT(C40:E42,$C$51:$E$53)+$G$51</f>
+        <v>46.6</v>
+      </c>
+      <c r="M41" s="1">
+        <f t="shared" si="44"/>
+        <v>50.199999999999996</v>
+      </c>
+      <c r="N41" s="1">
+        <f t="shared" si="44"/>
+        <v>53.8</v>
+      </c>
+      <c r="O41" s="1">
+        <f t="shared" si="44"/>
+        <v>57.4</v>
+      </c>
+      <c r="P41" s="1"/>
+      <c r="Q41" s="1"/>
+      <c r="R41" s="1"/>
+      <c r="S41" s="1"/>
+      <c r="T41" s="1"/>
+      <c r="U41" s="1"/>
+      <c r="V41" s="1"/>
+      <c r="W41" s="1"/>
+      <c r="X41" s="1"/>
+      <c r="Y41" s="1"/>
+      <c r="Z41" s="1"/>
+      <c r="AA41" s="1"/>
+      <c r="AB41" s="1"/>
+      <c r="AC41" s="1"/>
+    </row>
+    <row r="42" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B42" s="1">
+        <f>B41+7</f>
+        <v>14</v>
+      </c>
+      <c r="C42" s="1">
+        <f t="shared" si="38"/>
+        <v>15</v>
+      </c>
+      <c r="D42" s="1">
+        <f t="shared" si="39"/>
+        <v>16</v>
+      </c>
+      <c r="E42" s="1">
+        <f t="shared" si="40"/>
+        <v>17</v>
+      </c>
+      <c r="F42" s="1">
+        <f t="shared" si="41"/>
+        <v>18</v>
+      </c>
+      <c r="G42" s="1">
+        <f t="shared" si="42"/>
+        <v>19</v>
+      </c>
+      <c r="H42" s="1">
+        <f t="shared" si="43"/>
+        <v>20</v>
+      </c>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1">
+        <f t="shared" ref="K42:K45" si="45">SUMPRODUCT(B41:D43,$C$51:$E$53)+$G$51</f>
+        <v>68.199999999999989</v>
+      </c>
+      <c r="L42" s="1">
+        <f t="shared" ref="L42:L45" si="46">SUMPRODUCT(C41:E43,$C$51:$E$53)+$G$51</f>
+        <v>71.8</v>
+      </c>
+      <c r="M42" s="1">
+        <f t="shared" ref="M42:M45" si="47">SUMPRODUCT(D41:F43,$C$51:$E$53)+$G$51</f>
+        <v>75.400000000000006</v>
+      </c>
+      <c r="N42" s="1">
+        <f t="shared" ref="N42:N45" si="48">SUMPRODUCT(E41:G43,$C$51:$E$53)+$G$51</f>
+        <v>79</v>
+      </c>
+      <c r="O42" s="1">
+        <f t="shared" ref="O42:O45" si="49">SUMPRODUCT(F41:H43,$C$51:$E$53)+$G$51</f>
+        <v>82.6</v>
+      </c>
+      <c r="P42" s="1"/>
+      <c r="Q42" s="1"/>
+      <c r="R42" s="1"/>
+      <c r="S42" s="1">
+        <f>SUMPRODUCT(K41:M43,$L$51:$N$53)+$P$51</f>
+        <v>307</v>
+      </c>
+      <c r="T42" s="1">
+        <f t="shared" ref="T42:T44" si="50">SUMPRODUCT(L41:N43,$L$13:$N$15)+$P$13</f>
+        <v>319.95999999999998</v>
+      </c>
+      <c r="U42" s="1">
+        <f t="shared" ref="U42:U44" si="51">SUMPRODUCT(M41:O43,$L$13:$N$15)+$P$13</f>
+        <v>332.92</v>
+      </c>
+      <c r="V42" s="1"/>
+      <c r="W42" s="1"/>
+      <c r="X42" s="1">
+        <f>S42</f>
+        <v>307</v>
+      </c>
+      <c r="Y42" s="1"/>
+      <c r="Z42" s="1"/>
+      <c r="AA42" s="1">
+        <f t="array" ref="AA42:AA43">MMULT(TRANSPOSE(X53:Y61),X42:X50)</f>
+        <v>3696.12</v>
+      </c>
+      <c r="AB42" s="1">
+        <f>AA42+1</f>
+        <v>3697.12</v>
+      </c>
+      <c r="AC42" s="1">
+        <v>3700</v>
+      </c>
+    </row>
+    <row r="43" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B43" s="1">
+        <f>B42+7</f>
+        <v>21</v>
+      </c>
+      <c r="C43" s="1">
+        <f t="shared" si="38"/>
+        <v>22</v>
+      </c>
+      <c r="D43" s="1">
+        <f t="shared" si="39"/>
+        <v>23</v>
+      </c>
+      <c r="E43" s="1">
+        <f t="shared" si="40"/>
+        <v>24</v>
+      </c>
+      <c r="F43" s="1">
+        <f t="shared" si="41"/>
+        <v>25</v>
+      </c>
+      <c r="G43" s="1">
+        <f t="shared" si="42"/>
+        <v>26</v>
+      </c>
+      <c r="H43" s="1">
+        <f t="shared" si="43"/>
+        <v>27</v>
+      </c>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1">
+        <f t="shared" si="45"/>
+        <v>93.4</v>
+      </c>
+      <c r="L43" s="1">
+        <f t="shared" si="46"/>
+        <v>96.999999999999986</v>
+      </c>
+      <c r="M43" s="1">
+        <f t="shared" si="47"/>
+        <v>100.6</v>
+      </c>
+      <c r="N43" s="1">
+        <f t="shared" si="48"/>
+        <v>104.19999999999999</v>
+      </c>
+      <c r="O43" s="1">
+        <f t="shared" si="49"/>
+        <v>107.8</v>
+      </c>
+      <c r="P43" s="1"/>
+      <c r="Q43" s="1"/>
+      <c r="R43" s="1"/>
+      <c r="S43" s="1">
+        <f t="shared" ref="S43:S44" si="52">SUMPRODUCT(K42:M44,$L$13:$N$15)+$P$13</f>
+        <v>397.71999999999997</v>
+      </c>
+      <c r="T43" s="1">
+        <f t="shared" si="50"/>
+        <v>410.67999999999995</v>
+      </c>
+      <c r="U43" s="1">
+        <f t="shared" si="51"/>
+        <v>423.64</v>
+      </c>
+      <c r="V43" s="1"/>
+      <c r="W43" s="1"/>
+      <c r="X43" s="1">
+        <f t="shared" ref="X43:X44" si="53">S43</f>
+        <v>397.71999999999997</v>
+      </c>
+      <c r="Y43" s="1"/>
+      <c r="Z43" s="1"/>
+      <c r="AA43" s="1">
+        <v>3696.12</v>
+      </c>
+      <c r="AB43" s="1">
+        <f>AA43+1</f>
+        <v>3697.12</v>
+      </c>
+      <c r="AC43" s="1">
+        <v>3690</v>
+      </c>
+    </row>
+    <row r="44" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B44" s="1">
+        <f>B43+7</f>
+        <v>28</v>
+      </c>
+      <c r="C44" s="1">
+        <f t="shared" si="38"/>
+        <v>29</v>
+      </c>
+      <c r="D44" s="1">
+        <f t="shared" si="39"/>
+        <v>30</v>
+      </c>
+      <c r="E44" s="1">
+        <f t="shared" si="40"/>
+        <v>31</v>
+      </c>
+      <c r="F44" s="1">
+        <f t="shared" si="41"/>
+        <v>32</v>
+      </c>
+      <c r="G44" s="1">
+        <f t="shared" si="42"/>
+        <v>33</v>
+      </c>
+      <c r="H44" s="1">
+        <f t="shared" si="43"/>
+        <v>34</v>
+      </c>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="1">
+        <f t="shared" si="45"/>
+        <v>118.6</v>
+      </c>
+      <c r="L44" s="1">
+        <f t="shared" si="46"/>
+        <v>122.19999999999999</v>
+      </c>
+      <c r="M44" s="1">
+        <f t="shared" si="47"/>
+        <v>125.79999999999998</v>
+      </c>
+      <c r="N44" s="1">
+        <f t="shared" si="48"/>
+        <v>129.39999999999998</v>
+      </c>
+      <c r="O44" s="1">
+        <f t="shared" si="49"/>
+        <v>133</v>
+      </c>
+      <c r="P44" s="1"/>
+      <c r="Q44" s="1"/>
+      <c r="R44" s="1"/>
+      <c r="S44" s="1">
+        <f t="shared" si="52"/>
+        <v>488.43999999999994</v>
+      </c>
+      <c r="T44" s="1">
+        <f t="shared" si="50"/>
+        <v>501.4</v>
+      </c>
+      <c r="U44" s="1">
+        <f t="shared" si="51"/>
+        <v>514.3599999999999</v>
+      </c>
+      <c r="V44" s="1"/>
+      <c r="W44" s="1"/>
+      <c r="X44" s="1">
+        <f t="shared" si="53"/>
+        <v>488.43999999999994</v>
+      </c>
+      <c r="Y44" s="1"/>
+      <c r="Z44" s="1"/>
+      <c r="AA44" s="1"/>
+      <c r="AB44" s="1"/>
+      <c r="AC44" s="1"/>
+    </row>
+    <row r="45" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B45" s="1">
+        <f>B44+7</f>
+        <v>35</v>
+      </c>
+      <c r="C45" s="1">
+        <f t="shared" si="38"/>
+        <v>36</v>
+      </c>
+      <c r="D45" s="1">
+        <f t="shared" si="39"/>
+        <v>37</v>
+      </c>
+      <c r="E45" s="1">
+        <f t="shared" si="40"/>
+        <v>38</v>
+      </c>
+      <c r="F45" s="1">
+        <f t="shared" si="41"/>
+        <v>39</v>
+      </c>
+      <c r="G45" s="1">
+        <f t="shared" si="42"/>
+        <v>40</v>
+      </c>
+      <c r="H45" s="1">
+        <f t="shared" si="43"/>
+        <v>41</v>
+      </c>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1">
+        <f t="shared" si="45"/>
+        <v>143.79999999999998</v>
+      </c>
+      <c r="L45" s="1">
+        <f t="shared" si="46"/>
+        <v>147.39999999999998</v>
+      </c>
+      <c r="M45" s="1">
+        <f t="shared" si="47"/>
+        <v>151</v>
+      </c>
+      <c r="N45" s="1">
+        <f t="shared" si="48"/>
+        <v>154.6</v>
+      </c>
+      <c r="O45" s="1">
+        <f t="shared" si="49"/>
+        <v>158.19999999999999</v>
+      </c>
+      <c r="P45" s="1"/>
+      <c r="Q45" s="1"/>
+      <c r="R45" s="1"/>
+      <c r="S45" s="1"/>
+      <c r="T45" s="1"/>
+      <c r="U45" s="1"/>
+      <c r="V45" s="1"/>
+      <c r="W45" s="1"/>
+      <c r="X45" s="1">
+        <f>T42</f>
+        <v>319.95999999999998</v>
+      </c>
+      <c r="Y45" s="1"/>
+      <c r="Z45" s="1"/>
+      <c r="AA45" s="1"/>
+      <c r="AB45" s="1"/>
+      <c r="AC45" s="1"/>
+    </row>
+    <row r="46" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B46" s="1">
+        <f>B45+7</f>
+        <v>42</v>
+      </c>
+      <c r="C46" s="1">
+        <f t="shared" si="38"/>
+        <v>43</v>
+      </c>
+      <c r="D46" s="1">
+        <f t="shared" si="39"/>
+        <v>44</v>
+      </c>
+      <c r="E46" s="1">
+        <f t="shared" si="40"/>
+        <v>45</v>
+      </c>
+      <c r="F46" s="1">
+        <f t="shared" si="41"/>
+        <v>46</v>
+      </c>
+      <c r="G46" s="1">
+        <f t="shared" si="42"/>
+        <v>47</v>
+      </c>
+      <c r="H46" s="1">
+        <f t="shared" si="43"/>
+        <v>48</v>
+      </c>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
+      <c r="L46" s="1"/>
+      <c r="M46" s="1"/>
+      <c r="N46" s="1"/>
+      <c r="O46" s="1"/>
+      <c r="P46" s="1"/>
+      <c r="Q46" s="1"/>
+      <c r="R46" s="1"/>
+      <c r="S46" s="1"/>
+      <c r="T46" s="1"/>
+      <c r="U46" s="1"/>
+      <c r="V46" s="1"/>
+      <c r="W46" s="1"/>
+      <c r="X46" s="1">
+        <f t="shared" ref="X46:X47" si="54">T43</f>
+        <v>410.67999999999995</v>
+      </c>
+      <c r="Y46" s="1"/>
+      <c r="Z46" s="1"/>
+      <c r="AA46" s="1"/>
+      <c r="AB46" s="1"/>
+      <c r="AC46" s="1"/>
+    </row>
+    <row r="47" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+      <c r="L47" s="1"/>
+      <c r="M47" s="1"/>
+      <c r="N47" s="1"/>
+      <c r="O47" s="1"/>
+      <c r="P47" s="1"/>
+      <c r="Q47" s="1"/>
+      <c r="R47" s="1"/>
+      <c r="S47" s="1"/>
+      <c r="T47" s="1"/>
+      <c r="U47" s="1"/>
+      <c r="V47" s="1"/>
+      <c r="W47" s="1"/>
+      <c r="X47" s="1">
+        <f t="shared" si="54"/>
+        <v>501.4</v>
+      </c>
+      <c r="Y47" s="1"/>
+      <c r="Z47" s="1"/>
+      <c r="AA47" s="1"/>
+      <c r="AB47" s="1"/>
+      <c r="AC47" s="1"/>
+    </row>
+    <row r="48" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
+      <c r="L48" s="1"/>
+      <c r="M48" s="1"/>
+      <c r="N48" s="1"/>
+      <c r="O48" s="1"/>
+      <c r="P48" s="1"/>
+      <c r="Q48" s="1"/>
+      <c r="R48" s="1"/>
+      <c r="S48" s="1"/>
+      <c r="T48" s="1"/>
+      <c r="U48" s="1"/>
+      <c r="V48" s="1"/>
+      <c r="W48" s="1"/>
+      <c r="X48" s="1">
+        <f>U42</f>
+        <v>332.92</v>
+      </c>
+      <c r="Y48" s="1"/>
+      <c r="Z48" s="1"/>
+      <c r="AA48" s="1"/>
+      <c r="AB48" s="1"/>
+      <c r="AC48" s="1"/>
+    </row>
+    <row r="49" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
+      <c r="L49" s="1"/>
+      <c r="M49" s="1"/>
+      <c r="N49" s="1"/>
+      <c r="O49" s="1"/>
+      <c r="P49" s="1"/>
+      <c r="Q49" s="1"/>
+      <c r="R49" s="1"/>
+      <c r="S49" s="1"/>
+      <c r="T49" s="1"/>
+      <c r="U49" s="1"/>
+      <c r="V49" s="1"/>
+      <c r="W49" s="1"/>
+      <c r="X49" s="1">
+        <f t="shared" ref="X49:X50" si="55">U43</f>
+        <v>423.64</v>
+      </c>
+      <c r="Y49" s="1"/>
+      <c r="Z49" s="1"/>
+      <c r="AA49" s="1"/>
+      <c r="AB49" s="1"/>
+      <c r="AC49" s="1"/>
+    </row>
+    <row r="50" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
+      <c r="L50" s="1"/>
+      <c r="M50" s="1"/>
+      <c r="N50" s="1"/>
+      <c r="O50" s="1"/>
+      <c r="P50" s="1"/>
+      <c r="Q50" s="1"/>
+      <c r="R50" s="1"/>
+      <c r="S50" s="1"/>
+      <c r="T50" s="1"/>
+      <c r="U50" s="1"/>
+      <c r="V50" s="1"/>
+      <c r="W50" s="1"/>
+      <c r="X50" s="1">
+        <f t="shared" si="55"/>
+        <v>514.3599999999999</v>
+      </c>
+      <c r="Y50" s="1"/>
+      <c r="Z50" s="1"/>
+      <c r="AA50" s="1"/>
+      <c r="AB50" s="1">
+        <f>(AC42-AB42)*(AC42-AB42)</f>
+        <v>8.2944000000006284</v>
+      </c>
+      <c r="AC50" s="1"/>
+    </row>
+    <row r="51" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B51" s="1"/>
+      <c r="C51" s="1">
+        <v>0</v>
+      </c>
+      <c r="D51" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E51" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1">
+        <v>1</v>
+      </c>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
+      <c r="L51" s="1">
+        <v>0</v>
+      </c>
+      <c r="M51" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="N51" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="O51" s="1"/>
+      <c r="P51" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q51" s="1"/>
+      <c r="R51" s="1"/>
+      <c r="S51" s="1"/>
+      <c r="T51" s="1"/>
+      <c r="U51" s="1"/>
+      <c r="V51" s="1"/>
+      <c r="W51" s="1"/>
+      <c r="X51" s="1"/>
+      <c r="Y51" s="1"/>
+      <c r="Z51" s="1"/>
+      <c r="AA51" s="1"/>
+      <c r="AB51" s="1">
+        <f>(AC43-AB43)*(AC43-AB43)</f>
+        <v>50.694399999998446</v>
+      </c>
+      <c r="AC51" s="1"/>
+    </row>
+    <row r="52" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B52" s="1"/>
+      <c r="C52" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="D52" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="E52" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
+      <c r="L52" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="M52" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="N52" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="O52" s="1"/>
+      <c r="P52" s="1"/>
+      <c r="Q52" s="1"/>
+      <c r="R52" s="1"/>
+      <c r="S52" s="1"/>
+      <c r="T52" s="1"/>
+      <c r="U52" s="1"/>
+      <c r="V52" s="1"/>
+      <c r="W52" s="1"/>
+      <c r="X52" s="1"/>
+      <c r="Y52" s="1"/>
+      <c r="Z52" s="1"/>
+      <c r="AA52" s="1"/>
+      <c r="AB52" s="1">
+        <f>SUM(AB50:AB51)*0.5</f>
+        <v>29.494399999999537</v>
+      </c>
+      <c r="AC52" s="1"/>
+    </row>
+    <row r="53" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B53" s="1"/>
+      <c r="C53" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="D53" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="E53" s="1">
+        <v>0.79999999999999993</v>
+      </c>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
+      <c r="L53" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="M53" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="N53" s="1">
+        <v>0.79999999999999993</v>
+      </c>
+      <c r="O53" s="1"/>
+      <c r="P53" s="1"/>
+      <c r="Q53" s="1"/>
+      <c r="R53" s="1"/>
+      <c r="S53" s="1"/>
+      <c r="T53" s="1"/>
+      <c r="U53" s="1"/>
+      <c r="V53" s="1"/>
+      <c r="W53" s="1"/>
+      <c r="X53" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y53" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z53" s="1"/>
+      <c r="AA53" s="1"/>
+      <c r="AB53" s="1"/>
+      <c r="AC53" s="1"/>
+    </row>
+    <row r="54" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
+      <c r="L54" s="1"/>
+      <c r="M54" s="1"/>
+      <c r="N54" s="1"/>
+      <c r="O54" s="1"/>
+      <c r="P54" s="1"/>
+      <c r="Q54" s="1"/>
+      <c r="R54" s="1"/>
+      <c r="S54" s="1"/>
+      <c r="T54" s="1"/>
+      <c r="U54" s="1"/>
+      <c r="V54" s="1"/>
+      <c r="W54" s="1"/>
+      <c r="X54" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y54" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z54" s="1"/>
+      <c r="AA54" s="1"/>
+      <c r="AB54" s="1"/>
+      <c r="AC54" s="1"/>
+    </row>
+    <row r="55" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
+      <c r="K55" s="1"/>
+      <c r="L55" s="1"/>
+      <c r="M55" s="1"/>
+      <c r="N55" s="1"/>
+      <c r="O55" s="1"/>
+      <c r="P55" s="1"/>
+      <c r="Q55" s="1"/>
+      <c r="R55" s="1"/>
+      <c r="S55" s="1"/>
+      <c r="T55" s="1"/>
+      <c r="U55" s="1"/>
+      <c r="V55" s="1"/>
+      <c r="W55" s="1"/>
+      <c r="X55" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y55" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z55" s="1"/>
+      <c r="AA55" s="1">
+        <v>29.768633038399976</v>
+      </c>
+      <c r="AB55" s="1">
+        <v>29.228287438399128</v>
+      </c>
+      <c r="AC55" s="1">
+        <f>(AA55-AB55)/0.0002</f>
+        <v>2701.7280000042374</v>
+      </c>
+    </row>
+    <row r="56" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
+      <c r="K56" s="1"/>
+      <c r="L56" s="1"/>
+      <c r="M56" s="1"/>
+      <c r="N56" s="1"/>
+      <c r="O56" s="1"/>
+      <c r="P56" s="1"/>
+      <c r="Q56" s="1"/>
+      <c r="R56" s="1"/>
+      <c r="S56" s="1"/>
+      <c r="T56" s="1"/>
+      <c r="U56" s="1"/>
+      <c r="V56" s="1"/>
+      <c r="W56" s="1"/>
+      <c r="X56" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y56" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z56" s="1"/>
+      <c r="AA56" s="1"/>
+      <c r="AB56" s="1"/>
+      <c r="AC56" s="1"/>
+    </row>
+    <row r="57" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
+      <c r="K57" s="1"/>
+      <c r="L57" s="1"/>
+      <c r="M57" s="1"/>
+      <c r="N57" s="1"/>
+      <c r="O57" s="1"/>
+      <c r="P57" s="1"/>
+      <c r="Q57" s="1"/>
+      <c r="R57" s="1"/>
+      <c r="S57" s="1"/>
+      <c r="T57" s="1"/>
+      <c r="U57" s="1"/>
+      <c r="V57" s="1"/>
+      <c r="W57" s="1"/>
+      <c r="X57" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y57" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z57" s="1"/>
+      <c r="AA57" s="1"/>
+      <c r="AB57" s="1"/>
+      <c r="AC57" s="1"/>
+    </row>
+    <row r="58" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1"/>
+      <c r="K58" s="1"/>
+      <c r="L58" s="1"/>
+      <c r="M58" s="1"/>
+      <c r="N58" s="1"/>
+      <c r="O58" s="1"/>
+      <c r="P58" s="1"/>
+      <c r="Q58" s="1"/>
+      <c r="R58" s="1"/>
+      <c r="S58" s="1"/>
+      <c r="T58" s="1"/>
+      <c r="U58" s="1"/>
+      <c r="V58" s="1"/>
+      <c r="W58" s="1"/>
+      <c r="X58" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y58" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z58" s="1"/>
+      <c r="AA58" s="1"/>
+      <c r="AB58" s="1"/>
+      <c r="AC58" s="1"/>
+    </row>
+    <row r="59" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1"/>
+      <c r="K59" s="1"/>
+      <c r="L59" s="1"/>
+      <c r="M59" s="1"/>
+      <c r="N59" s="1"/>
+      <c r="O59" s="1"/>
+      <c r="P59" s="1"/>
+      <c r="Q59" s="1"/>
+      <c r="R59" s="1"/>
+      <c r="S59" s="1"/>
+      <c r="T59" s="1"/>
+      <c r="U59" s="1"/>
+      <c r="V59" s="1"/>
+      <c r="W59" s="1"/>
+      <c r="X59" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y59" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z59" s="1"/>
+      <c r="AA59" s="1"/>
+      <c r="AB59" s="1"/>
+      <c r="AC59" s="1"/>
+    </row>
+    <row r="60" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
+      <c r="K60" s="1"/>
+      <c r="L60" s="1"/>
+      <c r="M60" s="1"/>
+      <c r="N60" s="1"/>
+      <c r="O60" s="1"/>
+      <c r="P60" s="1"/>
+      <c r="Q60" s="1"/>
+      <c r="R60" s="1"/>
+      <c r="S60" s="1"/>
+      <c r="T60" s="1"/>
+      <c r="U60" s="1"/>
+      <c r="V60" s="1"/>
+      <c r="W60" s="1"/>
+      <c r="X60" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y60" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z60" s="1"/>
+      <c r="AA60" s="1"/>
+      <c r="AB60" s="1"/>
+      <c r="AC60" s="1"/>
+    </row>
+    <row r="61" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+      <c r="J61" s="1"/>
+      <c r="K61" s="1"/>
+      <c r="L61" s="1"/>
+      <c r="M61" s="1"/>
+      <c r="N61" s="1"/>
+      <c r="O61" s="1"/>
+      <c r="P61" s="1"/>
+      <c r="Q61" s="1"/>
+      <c r="R61" s="1"/>
+      <c r="S61" s="1"/>
+      <c r="T61" s="1"/>
+      <c r="U61" s="1"/>
+      <c r="V61" s="1"/>
+      <c r="W61" s="1"/>
+      <c r="X61" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y61" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z61" s="1"/>
+      <c r="AA61" s="1"/>
+      <c r="AB61" s="1"/>
+      <c r="AC61" s="1"/>
+    </row>
+    <row r="62" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+      <c r="J62" s="1"/>
+      <c r="K62" s="1"/>
+      <c r="L62" s="1"/>
+      <c r="M62" s="1"/>
+      <c r="N62" s="1"/>
+      <c r="O62" s="1"/>
+      <c r="P62" s="1"/>
+      <c r="Q62" s="1"/>
+      <c r="R62" s="1"/>
+      <c r="S62" s="1"/>
+      <c r="T62" s="1"/>
+      <c r="U62" s="1"/>
+      <c r="V62" s="1"/>
+      <c r="W62" s="1"/>
+      <c r="X62" s="1"/>
+      <c r="Y62" s="1"/>
+      <c r="Z62" s="1"/>
+      <c r="AA62" s="1"/>
+      <c r="AB62" s="1"/>
+      <c r="AC62" s="1"/>
+    </row>
+    <row r="63" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="1"/>
+      <c r="J63" s="1"/>
+      <c r="K63" s="1"/>
+      <c r="L63" s="1"/>
+      <c r="M63" s="1"/>
+      <c r="N63" s="1"/>
+      <c r="O63" s="1"/>
+      <c r="P63" s="1"/>
+      <c r="Q63" s="1"/>
+      <c r="R63" s="1"/>
+      <c r="S63" s="1"/>
+      <c r="T63" s="1"/>
+      <c r="U63" s="1"/>
+      <c r="V63" s="1"/>
+      <c r="W63" s="1"/>
+      <c r="X63" s="1"/>
+      <c r="Y63" s="1"/>
+      <c r="Z63" s="1"/>
+      <c r="AA63" s="1"/>
+      <c r="AB63" s="1"/>
+      <c r="AC63" s="1"/>
+    </row>
+    <row r="64" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
+      <c r="H64" s="1"/>
+      <c r="I64" s="1"/>
+      <c r="J64" s="1"/>
+      <c r="K64" s="1"/>
+      <c r="L64" s="1"/>
+      <c r="M64" s="1"/>
+      <c r="N64" s="1"/>
+      <c r="O64" s="1"/>
+      <c r="P64" s="1"/>
+      <c r="Q64" s="1"/>
+      <c r="R64" s="1"/>
+      <c r="S64" s="1"/>
+      <c r="T64" s="1"/>
+      <c r="U64" s="1"/>
+      <c r="V64" s="1"/>
+      <c r="W64" s="1"/>
+      <c r="X64" s="1"/>
+      <c r="Y64" s="1"/>
+      <c r="Z64" s="1"/>
+      <c r="AA64" s="1"/>
+      <c r="AB64" s="1"/>
+      <c r="AC64" s="1"/>
+    </row>
+    <row r="65" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+      <c r="J65" s="1"/>
+      <c r="K65" s="1"/>
+      <c r="L65" s="1"/>
+      <c r="M65" s="1"/>
+      <c r="N65" s="1"/>
+      <c r="O65" s="1"/>
+      <c r="P65" s="1"/>
+      <c r="Q65" s="1"/>
+      <c r="R65" s="1"/>
+      <c r="S65" s="1"/>
+      <c r="T65" s="1"/>
+      <c r="U65" s="1"/>
+      <c r="V65" s="1"/>
+      <c r="W65" s="1"/>
+      <c r="X65" s="1"/>
+      <c r="Y65" s="1"/>
+      <c r="Z65" s="1"/>
+      <c r="AA65" s="1"/>
+      <c r="AB65" s="1"/>
+      <c r="AC65" s="1"/>
+    </row>
+    <row r="66" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="1"/>
+      <c r="J66" s="1"/>
+      <c r="K66" s="1"/>
+      <c r="L66" s="1"/>
+      <c r="M66" s="1"/>
+      <c r="N66" s="1"/>
+      <c r="O66" s="1"/>
+      <c r="P66" s="1"/>
+      <c r="Q66" s="1"/>
+      <c r="R66" s="1"/>
+      <c r="S66" s="1"/>
+      <c r="T66" s="1"/>
+      <c r="U66" s="1"/>
+      <c r="V66" s="1"/>
+      <c r="W66" s="1"/>
+      <c r="X66" s="1"/>
+      <c r="Y66" s="1"/>
+      <c r="Z66" s="1"/>
+      <c r="AA66" s="1"/>
+      <c r="AB66" s="1"/>
+      <c r="AC66" s="1"/>
+    </row>
+    <row r="67" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
+      <c r="H67" s="1"/>
+      <c r="I67" s="1"/>
+      <c r="J67" s="1"/>
+      <c r="K67" s="1"/>
+      <c r="L67" s="1"/>
+      <c r="M67" s="1"/>
+      <c r="N67" s="1"/>
+      <c r="O67" s="1"/>
+      <c r="P67" s="1"/>
+      <c r="Q67" s="1"/>
+      <c r="R67" s="1"/>
+      <c r="S67" s="1"/>
+      <c r="T67" s="1"/>
+      <c r="U67" s="1"/>
+      <c r="V67" s="1"/>
+      <c r="W67" s="1"/>
+      <c r="X67" s="1"/>
+      <c r="Y67" s="1"/>
+      <c r="Z67" s="1"/>
+      <c r="AA67" s="1"/>
+      <c r="AB67" s="1"/>
+      <c r="AC67" s="1"/>
+    </row>
+    <row r="68" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
+      <c r="I68" s="1"/>
+      <c r="J68" s="1"/>
+      <c r="K68" s="1"/>
+      <c r="L68" s="1"/>
+      <c r="M68" s="1"/>
+      <c r="N68" s="1"/>
+      <c r="O68" s="1"/>
+      <c r="P68" s="1"/>
+      <c r="Q68" s="1"/>
+      <c r="R68" s="1"/>
+      <c r="S68" s="1"/>
+      <c r="T68" s="1"/>
+      <c r="U68" s="1"/>
+      <c r="V68" s="1"/>
+      <c r="W68" s="1"/>
+      <c r="X68" s="1"/>
+      <c r="Y68" s="1"/>
+      <c r="Z68" s="1"/>
+      <c r="AA68" s="1"/>
+      <c r="AB68" s="1"/>
+      <c r="AC68" s="1"/>
+    </row>
+    <row r="69" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
+      <c r="I69" s="1"/>
+      <c r="J69" s="1"/>
+      <c r="K69" s="1"/>
+      <c r="L69" s="1"/>
+      <c r="M69" s="1"/>
+      <c r="N69" s="1"/>
+      <c r="O69" s="1"/>
+      <c r="P69" s="1"/>
+      <c r="Q69" s="1"/>
+      <c r="R69" s="1"/>
+      <c r="S69" s="1"/>
+      <c r="T69" s="1"/>
+      <c r="U69" s="1"/>
+      <c r="V69" s="1"/>
+      <c r="W69" s="1"/>
+      <c r="X69" s="1"/>
+      <c r="Y69" s="1"/>
+      <c r="Z69" s="1"/>
+      <c r="AA69" s="1"/>
+      <c r="AB69" s="1"/>
+      <c r="AC69" s="1"/>
+    </row>
+    <row r="70" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
+      <c r="J70" s="1"/>
+      <c r="K70" s="1"/>
+      <c r="L70" s="1"/>
+      <c r="M70" s="1"/>
+      <c r="N70" s="1"/>
+      <c r="O70" s="1"/>
+      <c r="P70" s="1"/>
+      <c r="Q70" s="1"/>
+      <c r="R70" s="1"/>
+      <c r="S70" s="1"/>
+      <c r="T70" s="1"/>
+      <c r="U70" s="1"/>
+      <c r="V70" s="1"/>
+      <c r="W70" s="1"/>
+      <c r="X70" s="1"/>
+      <c r="Y70" s="1"/>
+      <c r="Z70" s="1"/>
+      <c r="AA70" s="1"/>
+      <c r="AB70" s="1"/>
+      <c r="AC70" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>